<commit_message>
Added test condition for BPA
Tested 41.5 cm BPA with Paracord. Recalibrated SLoadCell.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16EDEC8-3DAA-4DA9-86EF-722468385892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EBF171-FE10-4F3D-8E72-50AE960C2370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Force (lbs)</t>
   </si>
@@ -61,6 +61,42 @@
   </si>
   <si>
     <t>Max Strain</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>F'</t>
+  </si>
+  <si>
+    <t>Distance between crossmembers</t>
+  </si>
+  <si>
+    <t>Resting tendon length</t>
+  </si>
+  <si>
+    <t>Tendon material</t>
+  </si>
+  <si>
+    <t>yellow paracord</t>
+  </si>
+  <si>
+    <t>tendon length</t>
+  </si>
+  <si>
+    <t>tendon strain</t>
+  </si>
+  <si>
+    <t>Crossmember distance</t>
+  </si>
+  <si>
+    <t>*18.2 lbs pretensioned</t>
+  </si>
+  <si>
+    <t>*39.1 lbs pretensioned</t>
+  </si>
+  <si>
+    <t>**19.8 lbs after pressure removed</t>
   </si>
 </sst>
 </file>
@@ -104,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,6 +525,355 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.47653193350831147"/>
+                  <c:y val="3.1990740740740743E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'11.2 cm, no T'!$P$13:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'11.2 cm, no T'!$Q$13:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B1FA-49D5-A449-67ACA66A5EC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="797497728"/>
+        <c:axId val="797499392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="797497728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797499392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="797499392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797497728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -551,6 +937,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>NoTendon</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -573,122 +962,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="7.0021216097987754E-2"/>
-                  <c:y val="-0.58255431612715081"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln w="25400">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="25400" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.13200721784776903"/>
-                  <c:y val="-0.42262102653834938"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln w="15875">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'41.5 cm'!$F$6:$F$12</c:f>
@@ -753,6 +1026,119 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8626-428E-9C03-CBBFEA171991}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Paracord</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'41.5 cm'!$N$6:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.17391304347826086</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2463768115942254E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65217391304347827</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91304347826086951</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7536231884057969</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28985507246376835</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2608695652173913</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14492753623188384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8985507246377034E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43478260869565216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'41.5 cm'!$K$6:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>311.37551200000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>402.56405480000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>129.88807072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1171545600000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.482216000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>266.89329600000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>290.46887048000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>356.30255016000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>473.73560040000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>213.51463680000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8626-428E-9C03-CBBFEA171991}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1023,6 +1409,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1540,6 +1966,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2095,6 +3037,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3CA9DD5-4A9D-4226-426E-A44D46C13390}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2103,15 +3081,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2436,10 +3414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5D9837-CB16-4300-A1DA-BD967A7687F8}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +3425,7 @@
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2455,7 +3433,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2463,7 +3441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2472,7 +3450,7 @@
         <v>0.1607142857142857</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2492,7 +3470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>111</v>
       </c>
@@ -2515,7 +3493,7 @@
         <v>5.5555555555555365E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>107</v>
       </c>
@@ -2538,7 +3516,7 @@
         <v>0.27777777777777751</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>102</v>
       </c>
@@ -2561,7 +3539,7 @@
         <v>0.55555555555555569</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>98</v>
       </c>
@@ -2584,7 +3562,7 @@
         <v>0.7777777777777779</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>93</v>
       </c>
@@ -2605,6 +3583,30 @@
       <c r="F10">
         <f t="shared" si="1"/>
         <v>1.0555555555555554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>111</v>
+      </c>
+      <c r="Q13">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>415</v>
+      </c>
+      <c r="Q14">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -2616,34 +3618,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1">
         <v>415</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1">
+        <v>415</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>885</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <v>346</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>346</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>139</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2651,8 +3681,21 @@
         <f>1-B2/B1</f>
         <v>0.16626506024096388</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <f>1-J2/J1</f>
+        <v>0.16626506024096388</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2671,8 +3714,35 @@
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>414</v>
       </c>
@@ -2694,8 +3764,39 @@
         <f>E6/$B$3</f>
         <v>1.4492753623188184E-2</v>
       </c>
+      <c r="I6">
+        <v>403</v>
+      </c>
+      <c r="J6">
+        <v>70</v>
+      </c>
+      <c r="K6">
+        <f>J6* 4.4482216</f>
+        <v>311.37551200000001</v>
+      </c>
+      <c r="L6">
+        <v>620</v>
+      </c>
+      <c r="M6">
+        <f>1-I6/$B$1</f>
+        <v>2.8915662650602414E-2</v>
+      </c>
+      <c r="N6">
+        <f>M6/$B$3</f>
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="O6">
+        <v>885</v>
+      </c>
+      <c r="P6">
+        <v>139</v>
+      </c>
+      <c r="Q6">
+        <f>P6/$N$2-1</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>407</v>
       </c>
@@ -2717,8 +3818,42 @@
         <f>E7/$B$3</f>
         <v>0.11594202898550747</v>
       </c>
+      <c r="I7">
+        <v>410</v>
+      </c>
+      <c r="J7">
+        <v>90.5</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K16" si="0">J7* 4.4482216</f>
+        <v>402.56405480000001</v>
+      </c>
+      <c r="L7">
+        <v>620</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M12" si="1">1-I7/$B$1</f>
+        <v>1.2048192771084376E-2</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:N16" si="2">M7/$B$3</f>
+        <v>7.2463768115942254E-2</v>
+      </c>
+      <c r="O7">
+        <v>895</v>
+      </c>
+      <c r="P7">
+        <v>143</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q16" si="3">P7/$N$2-1</f>
+        <v>2.877697841726623E-2</v>
+      </c>
+      <c r="R7" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>402</v>
       </c>
@@ -2726,7 +3861,7 @@
         <v>62</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C12" si="0">B8* 4.4482216</f>
+        <f t="shared" ref="C8:C12" si="4">B8* 4.4482216</f>
         <v>275.78973919999999</v>
       </c>
       <c r="D8">
@@ -2737,11 +3872,42 @@
         <v>3.1325301204819245E-2</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F14" si="1">E8/$B$3</f>
+        <f t="shared" ref="F8:F12" si="5">E8/$B$3</f>
         <v>0.18840579710144906</v>
       </c>
+      <c r="I8">
+        <v>370</v>
+      </c>
+      <c r="J8">
+        <v>29.2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>129.88807072</v>
+      </c>
+      <c r="L8">
+        <v>620</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.10843373493975905</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>0.65217391304347827</v>
+      </c>
+      <c r="O8">
+        <v>850</v>
+      </c>
+      <c r="P8">
+        <v>150</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>7.9136690647481966E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>387</v>
       </c>
@@ -2749,22 +3915,53 @@
         <v>45</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>200.169972</v>
       </c>
       <c r="D9">
         <v>620</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E14" si="2">1-A9/$B$1</f>
+        <f t="shared" ref="E9:E12" si="6">1-A9/$B$1</f>
         <v>6.7469879518072262E-2</v>
       </c>
       <c r="F9">
         <f>E9/$B$3</f>
         <v>0.40579710144927517</v>
       </c>
+      <c r="I9">
+        <v>352</v>
+      </c>
+      <c r="J9">
+        <v>1.6</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>7.1171545600000004</v>
+      </c>
+      <c r="L9">
+        <v>620</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>0.15180722891566267</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>0.91304347826086951</v>
+      </c>
+      <c r="O9">
+        <v>820</v>
+      </c>
+      <c r="P9">
+        <v>139</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>368</v>
       </c>
@@ -2772,22 +3969,53 @@
         <v>23.2</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>103.19874111999999</v>
       </c>
       <c r="D10">
         <v>620</v>
       </c>
       <c r="E10">
+        <f t="shared" si="6"/>
+        <v>0.11325301204819282</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="5"/>
+        <v>0.68115942028985532</v>
+      </c>
+      <c r="I10">
+        <v>363</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>44.482216000000001</v>
+      </c>
+      <c r="L10">
+        <v>620</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>0.12530120481927709</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="2"/>
-        <v>0.11325301204819282</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0.68115942028985532</v>
+        <v>0.7536231884057969</v>
+      </c>
+      <c r="O10">
+        <v>830</v>
+      </c>
+      <c r="P10">
+        <v>140</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>7.194244604316502E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>352</v>
       </c>
@@ -2795,22 +4023,53 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>40.92363872</v>
       </c>
       <c r="D11">
         <v>620</v>
       </c>
       <c r="E11">
+        <f t="shared" si="6"/>
+        <v>0.15180722891566267</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="5"/>
+        <v>0.91304347826086951</v>
+      </c>
+      <c r="I11">
+        <v>395</v>
+      </c>
+      <c r="J11">
+        <v>60</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>266.89329600000002</v>
+      </c>
+      <c r="L11">
+        <v>620</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>4.8192771084337394E-2</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="2"/>
-        <v>0.15180722891566267</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0.91304347826086951</v>
+        <v>0.28985507246376835</v>
+      </c>
+      <c r="O11">
+        <v>879</v>
+      </c>
+      <c r="P11">
+        <v>142</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>2.1582733812949728E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>346</v>
       </c>
@@ -2818,19 +4077,188 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D12">
         <v>620</v>
       </c>
       <c r="E12">
+        <f t="shared" si="6"/>
+        <v>0.16626506024096388</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>397</v>
+      </c>
+      <c r="J12">
+        <v>65.3</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>290.46887048000002</v>
+      </c>
+      <c r="L12">
+        <v>620</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>4.3373493975903621E-2</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="2"/>
-        <v>0.16626506024096388</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="O12">
+        <v>881</v>
+      </c>
+      <c r="P12">
+        <v>142</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>2.1582733812949728E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>405</v>
+      </c>
+      <c r="J13">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>356.30255016000001</v>
+      </c>
+      <c r="L13">
+        <v>620</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13:M15" si="7">1-I13/$B$1</f>
+        <v>2.4096385542168641E-2</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>0.14492753623188384</v>
+      </c>
+      <c r="O13">
+        <v>890</v>
+      </c>
+      <c r="P13">
+        <v>143</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="3"/>
+        <v>2.877697841726623E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>413</v>
+      </c>
+      <c r="J14">
+        <v>106.5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>473.73560040000001</v>
+      </c>
+      <c r="L14">
+        <v>620</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>4.8192771084337727E-3</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>2.8985507246377034E-2</v>
+      </c>
+      <c r="O14">
+        <v>904</v>
+      </c>
+      <c r="P14">
+        <v>145</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="3"/>
+        <v>4.3165467625899234E-2</v>
+      </c>
+      <c r="R14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>385</v>
+      </c>
+      <c r="J15">
+        <v>48</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>213.51463680000001</v>
+      </c>
+      <c r="L15">
+        <v>620</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>7.2289156626506035E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="O15">
+        <v>870</v>
+      </c>
+      <c r="P15">
+        <v>143</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="3"/>
+        <v>2.877697841726623E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>375</v>
+      </c>
+      <c r="J16">
+        <v>37.9</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>168.58759864000001</v>
+      </c>
+      <c r="L16">
+        <v>620</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16" si="8">1-I16/$B$1</f>
+        <v>9.6385542168674676E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>0.57971014492753603</v>
+      </c>
+      <c r="O16">
+        <v>860</v>
+      </c>
+      <c r="P16">
+        <v>143</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="3"/>
+        <v>2.877697841726623E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added HX711 library for Matlab
Reinstalled MATLAB. Installed Matlab HX711 library to use with Arduino add on. It works. Added another test on the 41.5 cm BPA with it using bicycle brake cable.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EBF171-FE10-4F3D-8E72-50AE960C2370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410082A1-9485-4272-9E9B-D4B96C03DEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Force (lbs)</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>**19.8 lbs after pressure removed</t>
+  </si>
+  <si>
+    <t>Bicycle brake cable</t>
   </si>
 </sst>
 </file>
@@ -930,7 +933,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9247594050743664E-2"/>
+          <c:y val="0.14463917525773196"/>
+          <c:w val="0.87437751531058616"/>
+          <c:h val="0.79282382227994697"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1139,6 +1152,107 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-8626-428E-9C03-CBBFEA171991}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Brake Cable</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'41.5 cm'!$N$23:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.22368421052631557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10526315789473707</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98684210526315796</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84210526315789469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69736842105263142</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64473684210526327</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40789473684210498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'41.5 cm'!$K$23:$K$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>311.37551200000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>389.66421215999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.120554</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88964432000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.412653599999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.88127184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138.33969176000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>236.20056696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EA8D-4D5F-890A-792BC3EFF0E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3501,7 +3615,7 @@
         <v>56.8</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C13" si="0">B7* 4.4482216</f>
+        <f t="shared" ref="C7:C10" si="0">B7* 4.4482216</f>
         <v>252.65898687999999</v>
       </c>
       <c r="D7">
@@ -3512,7 +3626,7 @@
         <v>4.4642857142857095E-2</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F13" si="1">E7/$B$3</f>
+        <f t="shared" ref="F7:F10" si="1">E7/$B$3</f>
         <v>0.27777777777777751</v>
       </c>
     </row>
@@ -3531,7 +3645,7 @@
         <v>620</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E14" si="2">1-A8/$B$1</f>
+        <f t="shared" ref="E8:E10" si="2">1-A8/$B$1</f>
         <v>8.9285714285714302E-2</v>
       </c>
       <c r="F8">
@@ -3618,10 +3732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3778,11 +3892,11 @@
         <v>620</v>
       </c>
       <c r="M6">
-        <f>1-I6/$B$1</f>
+        <f>1-I6/$J$1</f>
         <v>2.8915662650602414E-2</v>
       </c>
       <c r="N6">
-        <f>M6/$B$3</f>
+        <f>M6/$J$3</f>
         <v>0.17391304347826086</v>
       </c>
       <c r="O6">
@@ -3832,11 +3946,11 @@
         <v>620</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M12" si="1">1-I7/$B$1</f>
+        <f t="shared" ref="M7:M16" si="1">1-I7/$J$1</f>
         <v>1.2048192771084376E-2</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N16" si="2">M7/$B$3</f>
+        <f t="shared" ref="N7:N16" si="2">M7/$J$3</f>
         <v>7.2463768115942254E-2</v>
       </c>
       <c r="O7">
@@ -4138,7 +4252,7 @@
         <v>620</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13:M15" si="7">1-I13/$B$1</f>
+        <f t="shared" si="1"/>
         <v>2.4096385542168641E-2</v>
       </c>
       <c r="N13">
@@ -4171,7 +4285,7 @@
         <v>620</v>
       </c>
       <c r="M14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>4.8192771084337727E-3</v>
       </c>
       <c r="N14">
@@ -4210,7 +4324,7 @@
         <v>620</v>
       </c>
       <c r="M15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>7.2289156626506035E-2</v>
       </c>
       <c r="N15">
@@ -4243,7 +4357,7 @@
         <v>620</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16" si="8">1-I16/$B$1</f>
+        <f t="shared" si="1"/>
         <v>9.6385542168674676E-2</v>
       </c>
       <c r="N16">
@@ -4259,6 +4373,342 @@
       <c r="Q16">
         <f t="shared" si="3"/>
         <v>2.877697841726623E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="9:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>416</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="19" spans="9:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>340</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20">
+        <f>1-J19/J18</f>
+        <v>0.18269230769230771</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="9:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>399</v>
+      </c>
+      <c r="J23">
+        <v>70</v>
+      </c>
+      <c r="K23">
+        <f>J23* 4.4482216</f>
+        <v>311.37551200000001</v>
+      </c>
+      <c r="L23">
+        <v>620</v>
+      </c>
+      <c r="M23">
+        <f>1-I23/$J$18</f>
+        <v>4.0865384615384581E-2</v>
+      </c>
+      <c r="N23">
+        <f>M23/$J$20</f>
+        <v>0.22368421052631557</v>
+      </c>
+      <c r="O23">
+        <v>815</v>
+      </c>
+      <c r="P23">
+        <v>104</v>
+      </c>
+      <c r="Q23">
+        <f>P23/$N$19-1</f>
+        <v>1.9607843137254832E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>408</v>
+      </c>
+      <c r="J24">
+        <v>87.6</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ref="K24:K33" si="7">J24* 4.4482216</f>
+        <v>389.66421215999998</v>
+      </c>
+      <c r="L24">
+        <v>620</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M33" si="8">1-I24/$J$18</f>
+        <v>1.9230769230769273E-2</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ref="N24:N33" si="9">M24/$J$20</f>
+        <v>0.10526315789473707</v>
+      </c>
+      <c r="O24">
+        <v>825</v>
+      </c>
+      <c r="P24">
+        <v>103</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" ref="Q24:Q33" si="10">P24/$N$19-1</f>
+        <v>9.8039215686274161E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>341</v>
+      </c>
+      <c r="J25">
+        <v>2.5</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="7"/>
+        <v>11.120554</v>
+      </c>
+      <c r="L25">
+        <v>620</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="8"/>
+        <v>0.18028846153846156</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="9"/>
+        <v>0.98684210526315796</v>
+      </c>
+      <c r="O25">
+        <v>759</v>
+      </c>
+      <c r="P25">
+        <v>103</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="10"/>
+        <v>9.8039215686274161E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>340</v>
+      </c>
+      <c r="J26">
+        <v>0.2</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="7"/>
+        <v>0.88964432000000004</v>
+      </c>
+      <c r="L26">
+        <v>620</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="8"/>
+        <v>0.18269230769230771</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>759</v>
+      </c>
+      <c r="P26">
+        <v>103</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="10"/>
+        <v>9.8039215686274161E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>352</v>
+      </c>
+      <c r="J27">
+        <v>21</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="7"/>
+        <v>93.412653599999999</v>
+      </c>
+      <c r="L27">
+        <v>620</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="8"/>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="9"/>
+        <v>0.84210526315789469</v>
+      </c>
+      <c r="O27">
+        <v>774</v>
+      </c>
+      <c r="P27">
+        <v>103</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="10"/>
+        <v>9.8039215686274161E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>363</v>
+      </c>
+      <c r="J28">
+        <v>27.4</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
+        <v>121.88127184</v>
+      </c>
+      <c r="L28">
+        <v>620</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="8"/>
+        <v>0.12740384615384615</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="9"/>
+        <v>0.69736842105263142</v>
+      </c>
+      <c r="O28">
+        <v>782</v>
+      </c>
+      <c r="P28">
+        <v>105</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="10"/>
+        <v>2.9411764705882248E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>367</v>
+      </c>
+      <c r="J29">
+        <v>31.1</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
+        <v>138.33969176000002</v>
+      </c>
+      <c r="L29">
+        <v>620</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="8"/>
+        <v>0.11778846153846156</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="9"/>
+        <v>0.64473684210526327</v>
+      </c>
+      <c r="O29">
+        <v>786</v>
+      </c>
+      <c r="P29">
+        <v>104</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="10"/>
+        <v>1.9607843137254832E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>385</v>
+      </c>
+      <c r="J30">
+        <v>53.1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="7"/>
+        <v>236.20056696</v>
+      </c>
+      <c r="L30">
+        <v>620</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="8"/>
+        <v>7.4519230769230727E-2</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="9"/>
+        <v>0.40789473684210498</v>
+      </c>
+      <c r="O30">
+        <v>806</v>
+      </c>
+      <c r="P30">
+        <v>105</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="10"/>
+        <v>2.9411764705882248E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified README for functions
Added the rest of the functions and their descriptions. Added a missing data point to straightforcetest graph. Tried to modify Alex's equation parameters to get the correct ForceStrainTable.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35771CA-9BD8-4CC2-99AE-0EBE247CA065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE892C17-9AF2-4AE3-8E5D-A3EF3A81AE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -1046,9 +1046,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Paracord</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -1073,10 +1070,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'41.5 cm'!$N$6:$N$15</c:f>
+              <c:f>'41.5 cm'!$N$6:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.17391304347826086</c:v>
                 </c:pt>
@@ -1106,16 +1103,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.43478260869565216</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57971014492753603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'41.5 cm'!$K$6:$K$15</c:f>
+              <c:f>'41.5 cm'!$K$6:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>311.37551200000001</c:v>
                 </c:pt>
@@ -1145,6 +1145,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>213.51463680000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>168.58759864000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4822,8 +4825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5810,8 +5813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050AE67D-A238-4925-A0DE-87F77397D646}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5908,11 +5911,11 @@
         <v>620</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E18" si="0">1-A7/$B$1</f>
+        <f t="shared" ref="E7:E16" si="0">1-A7/$B$1</f>
         <v>0.15164835164835166</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F18" si="1">E7/$B$3</f>
+        <f t="shared" ref="F7:F16" si="1">E7/$B$3</f>
         <v>0.95833333333333348</v>
       </c>
     </row>
@@ -6045,7 +6048,7 @@
         <v>58.9</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C18" si="2">B14*4.4482216</f>
+        <f t="shared" ref="C14:C16" si="2">B14*4.4482216</f>
         <v>262.00025224000001</v>
       </c>
       <c r="D14">

</xml_diff>

<commit_message>
Took two more data measurements
the 45.5cm BPA might be finished.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE892C17-9AF2-4AE3-8E5D-A3EF3A81AE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BF07A5-F320-4FEF-B2EE-2380452B2255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -1559,10 +1559,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'45.5 cm'!$F$6:$F$15</c:f>
+              <c:f>'45.5 cm'!$F$6:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666665</c:v>
                 </c:pt>
@@ -1592,16 +1592,25 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.23611111111111099</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13888888888888912</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1666666666666519E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.9444444444444198E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'45.5 cm'!$C$6:$C$15</c:f>
+              <c:f>'45.5 cm'!$C$6:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>26</c:v>
                 </c:pt>
@@ -1631,6 +1640,15 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>335.39590864000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>407.01227640000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>435.92571680000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>404.78816560000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4825,7 +4843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -5813,8 +5831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050AE67D-A238-4925-A0DE-87F77397D646}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5911,11 +5929,11 @@
         <v>620</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E16" si="0">1-A7/$B$1</f>
+        <f t="shared" ref="E7:E18" si="0">1-A7/$B$1</f>
         <v>0.15164835164835166</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F16" si="1">E7/$B$3</f>
+        <f t="shared" ref="F7:F18" si="1">E7/$B$3</f>
         <v>0.95833333333333348</v>
       </c>
     </row>
@@ -6048,7 +6066,7 @@
         <v>58.9</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C16" si="2">B14*4.4482216</f>
+        <f t="shared" ref="C14:C18" si="2">B14*4.4482216</f>
         <v>262.00025224000001</v>
       </c>
       <c r="D14">
@@ -6118,19 +6136,80 @@
         <v>695</v>
       </c>
     </row>
-    <row r="18" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>452</v>
+      </c>
+      <c r="B17">
+        <v>98</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>435.92571680000003</v>
+      </c>
+      <c r="D17">
+        <v>620</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>6.59340659340657E-3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666519E-2</v>
+      </c>
+      <c r="G17">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>450</v>
+      </c>
+      <c r="B18">
+        <v>91</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>404.78816560000001</v>
+      </c>
+      <c r="D18">
+        <v>620</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.098901098901095E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>6.9444444444444198E-2</v>
+      </c>
+      <c r="G18">
+        <v>700</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>620</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>620</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="22" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>

</xml_diff>

<commit_message>
Took more data for 49 cm BPA
Also created a hello world sketch. Having a hard time loading HX711 libraries in Matlab but it seems to be a problem with the WS4 computer because data was collected on my laptop.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BF07A5-F320-4FEF-B2EE-2380452B2255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0172E5F1-3793-47F9-A089-7DEE97433ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
     <sheet name="41.5 cm" sheetId="1" r:id="rId2"/>
     <sheet name="45.5 cm" sheetId="4" r:id="rId3"/>
+    <sheet name="49.0 cm" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
   <si>
     <t>Force (lbs)</t>
   </si>
@@ -101,6 +102,24 @@
   </si>
   <si>
     <t>Bicycle brake cable</t>
+  </si>
+  <si>
+    <t>*14.6 lbs pretension, 458 mm before inflation (i.e. stretched</t>
+  </si>
+  <si>
+    <t>*Had to switch from Matlab app to Arduino "calibration factor" sketch</t>
+  </si>
+  <si>
+    <t>*free hanging</t>
+  </si>
+  <si>
+    <t>*17 N pretension, part broke</t>
+  </si>
+  <si>
+    <t>*11.23 N pretension</t>
+  </si>
+  <si>
+    <t>*horizontal</t>
   </si>
 </sst>
 </file>
@@ -1559,10 +1578,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'45.5 cm'!$F$6:$F$18</c:f>
+              <c:f>'45.5 cm'!$F$6:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666665</c:v>
                 </c:pt>
@@ -1601,16 +1620,31 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6.9444444444444198E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5555555555555358E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.1666666666666519E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.13888888888888912</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.29166666666666635</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.47222222222222199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'45.5 cm'!$C$6:$C$18</c:f>
+              <c:f>'45.5 cm'!$C$6:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>26</c:v>
                 </c:pt>
@@ -1649,6 +1683,21 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>404.78816560000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>408.34674288000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>504.42832944000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>335.39590864000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>257.9968528</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>203.28372712000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1763,6 +1812,554 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-87E5-49F2-84EB-3DCDDBEDE0EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="406590880"/>
+        <c:axId val="406592960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="406590880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406592960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="406592960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406590880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Force vs. Relative Strain, 49.0 cm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9247594050743664E-2"/>
+          <c:y val="0.14463917525773196"/>
+          <c:w val="0.87437751531058616"/>
+          <c:h val="0.79282382227994697"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'49.0 cm'!$F$6:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.92391304347826053</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.934782608695652</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.0869565217391432E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.347826086956514E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16304347826086971</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11956521739130457</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.20652173913043487</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26086956521739141</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32608695652173886</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3695652173913046</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.434782608695652</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.51086956521739146</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.565217391304348</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.684782608695652</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.70652173913043481</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.78260869565217372</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.83695652173913027</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.88043478260869545</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.94565217391304346</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.98913043478260854</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'49.0 cm'!$C$6:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EBE3-423A-A3B9-68F4C1F44BDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Paracord</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'49.0 cm'!$N$6:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'49.0 cm'!$K$6:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EBE3-423A-A3B9-68F4C1F44BDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Brake Cable</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'49.0 cm'!$N$23:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'49.0 cm'!$K$23:$K$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EBE3-423A-A3B9-68F4C1F44BDA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2113,6 +2710,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3662,6 +4299,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4301,16 +5454,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4318,6 +5471,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBA602F7-D45C-4D95-B5CB-2E6CA5F0F485}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{982C00CA-6616-41F5-A4BF-4F315A7F5C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4843,7 +6039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -5829,10 +7025,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050AE67D-A238-4925-A0DE-87F77397D646}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5929,11 +7125,11 @@
         <v>620</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E18" si="0">1-A7/$B$1</f>
+        <f t="shared" ref="E7:E24" si="0">1-A7/$B$1</f>
         <v>0.15164835164835166</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F18" si="1">E7/$B$3</f>
+        <f t="shared" ref="F7:F24" si="1">E7/$B$3</f>
         <v>0.95833333333333348</v>
       </c>
     </row>
@@ -6057,6 +7253,9 @@
       <c r="G13">
         <v>665</v>
       </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -6066,7 +7265,7 @@
         <v>58.9</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C18" si="2">B14*4.4482216</f>
+        <f t="shared" ref="C14:C24" si="2">B14*4.4482216</f>
         <v>262.00025224000001</v>
       </c>
       <c r="D14">
@@ -6191,25 +7390,115 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>451</v>
+      </c>
+      <c r="B19">
+        <v>91.8</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>408.34674288000002</v>
+      </c>
       <c r="D19">
         <v>620</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>8.79120879120876E-3</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555358E-2</v>
+      </c>
+      <c r="G19">
+        <v>700</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>458</v>
+      </c>
+      <c r="B20">
+        <v>113.4</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>504.42832944000003</v>
+      </c>
       <c r="D20">
         <v>620</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>-6.59340659340657E-3</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>-4.1666666666666519E-2</v>
+      </c>
+      <c r="G20">
+        <v>706</v>
+      </c>
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>445</v>
+      </c>
+      <c r="B21">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>335.39590864000002</v>
+      </c>
       <c r="D21">
         <v>620</v>
       </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>2.1978021978022011E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0.13888888888888912</v>
+      </c>
+      <c r="G21">
+        <v>692</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>434</v>
+      </c>
+      <c r="B22">
+        <v>58</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>257.9968528</v>
+      </c>
+      <c r="D22">
+        <v>620</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>4.6153846153846101E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0.29166666666666635</v>
+      </c>
+      <c r="G22">
+        <v>681</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -6220,6 +7509,588 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>421</v>
+      </c>
+      <c r="B23">
+        <v>45.7</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>203.28372712000001</v>
+      </c>
+      <c r="D23">
+        <v>620</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>7.4725274725274682E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="G23">
+        <v>670</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C902C6E6-059B-43BE-A924-BB7C80CB41D4}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>490</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>398</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>1-B2/B1</f>
+        <v>0.18775510204081636</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>405</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>618</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E26" si="0">1-A6/$B$1</f>
+        <v>0.17346938775510201</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F26" si="1">E6/$B$3</f>
+        <v>0.92391304347826053</v>
+      </c>
+      <c r="G6">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>404</v>
+      </c>
+      <c r="C7">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D7">
+        <v>618</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.17551020408163265</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.934782608695652</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>491</v>
+      </c>
+      <c r="C8">
+        <v>464</v>
+      </c>
+      <c r="D8">
+        <v>620</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-2.0408163265306367E-3</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>-1.0869565217391432E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>486</v>
+      </c>
+      <c r="C9">
+        <v>433</v>
+      </c>
+      <c r="D9">
+        <v>616</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>8.1632653061224358E-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4.347826086956514E-2</v>
+      </c>
+      <c r="G9">
+        <v>737</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>475</v>
+      </c>
+      <c r="C10">
+        <v>320</v>
+      </c>
+      <c r="D10">
+        <v>618</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3.0612244897959218E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.16304347826086971</v>
+      </c>
+      <c r="G10">
+        <v>724</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>479</v>
+      </c>
+      <c r="C11">
+        <v>356</v>
+      </c>
+      <c r="D11">
+        <v>620</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.2448979591836782E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.11956521739130457</v>
+      </c>
+      <c r="G11">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>471</v>
+      </c>
+      <c r="C12">
+        <v>300</v>
+      </c>
+      <c r="D12">
+        <v>618</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3.8775510204081653E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.20652173913043487</v>
+      </c>
+      <c r="G12">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>466</v>
+      </c>
+      <c r="C13">
+        <v>268</v>
+      </c>
+      <c r="D13">
+        <v>617</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>4.8979591836734726E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.26086956521739141</v>
+      </c>
+      <c r="G13">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>460</v>
+      </c>
+      <c r="C14">
+        <v>241</v>
+      </c>
+      <c r="D14">
+        <v>617</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>6.1224489795918324E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.32608695652173886</v>
+      </c>
+      <c r="G14">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>456</v>
+      </c>
+      <c r="C15">
+        <v>215</v>
+      </c>
+      <c r="D15">
+        <v>617</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>6.9387755102040871E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.3695652173913046</v>
+      </c>
+      <c r="G15">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>450</v>
+      </c>
+      <c r="C16">
+        <v>194</v>
+      </c>
+      <c r="D16">
+        <v>617</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>8.1632653061224469E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.434782608695652</v>
+      </c>
+      <c r="G16">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>443</v>
+      </c>
+      <c r="C17">
+        <v>165</v>
+      </c>
+      <c r="D17">
+        <v>617</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>9.5918367346938815E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.51086956521739146</v>
+      </c>
+      <c r="G17">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>438</v>
+      </c>
+      <c r="C18">
+        <v>144</v>
+      </c>
+      <c r="D18">
+        <v>617</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.10612244897959189</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.565217391304348</v>
+      </c>
+      <c r="G18">
+        <v>685</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>427</v>
+      </c>
+      <c r="C19">
+        <v>107</v>
+      </c>
+      <c r="D19">
+        <v>617</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.12857142857142856</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.684782608695652</v>
+      </c>
+      <c r="G19">
+        <v>675</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>425</v>
+      </c>
+      <c r="C20">
+        <v>97</v>
+      </c>
+      <c r="D20">
+        <v>617</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.13265306122448983</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0.70652173913043481</v>
+      </c>
+      <c r="G20">
+        <v>670</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>418</v>
+      </c>
+      <c r="C21">
+        <v>75</v>
+      </c>
+      <c r="D21">
+        <v>617</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.14693877551020407</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0.78260869565217372</v>
+      </c>
+      <c r="G21">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>413</v>
+      </c>
+      <c r="C22">
+        <v>58</v>
+      </c>
+      <c r="D22">
+        <v>617</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.15714285714285714</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0.83695652173913027</v>
+      </c>
+      <c r="G22">
+        <v>661</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>409</v>
+      </c>
+      <c r="C23">
+        <v>45</v>
+      </c>
+      <c r="D23">
+        <v>617</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.16530612244897958</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.88043478260869545</v>
+      </c>
+      <c r="G23">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>403</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>617</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.17755102040816328</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0.94565217391304346</v>
+      </c>
+      <c r="G24">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>399</v>
+      </c>
+      <c r="C25">
+        <v>2.29</v>
+      </c>
+      <c r="D25">
+        <v>617</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.18571428571428572</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0.98913043478260854</v>
+      </c>
+      <c r="G25">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>398</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.18775510204081636</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Results for 52 cm BPA
Matlab HX711 app works now. I think the library for it under one of the HX711 v3.0 folder is corrupt. Will replace with working.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0172E5F1-3793-47F9-A089-7DEE97433ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DDCD83-ED74-48D5-A8E8-628771204992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
     <sheet name="41.5 cm" sheetId="1" r:id="rId2"/>
     <sheet name="45.5 cm" sheetId="4" r:id="rId3"/>
     <sheet name="49.0 cm" sheetId="5" r:id="rId4"/>
+    <sheet name="51.8 cm" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
   <si>
     <t>Force (lbs)</t>
   </si>
@@ -120,6 +121,15 @@
   </si>
   <si>
     <t>*horizontal</t>
+  </si>
+  <si>
+    <t>*pushed, slight bend in BPA, recorded distance is vertical (not path length)</t>
+  </si>
+  <si>
+    <t>*15.6 N pretension</t>
+  </si>
+  <si>
+    <t>*89 N pretension</t>
   </si>
 </sst>
 </file>
@@ -2550,6 +2560,611 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Force vs. Relative Strain, 49.0 cm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9247594050743664E-2"/>
+          <c:y val="0.14463917525773196"/>
+          <c:w val="0.87437751531058616"/>
+          <c:h val="0.79282382227994697"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.21563298337707787"/>
+                  <c:y val="-9.7590769903761948E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'51.8 cm'!$F$6:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0116279069767442</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0348837209302324</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90697674418604668</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4883720930232488E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13953488372092995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23255813953488391</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33720930232558138</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47674418604651136</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91860465116279089</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.81395348837209269</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.69767441860465107</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.61627906976744196</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.52325581395348864</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3255813953488327E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.9767441860464977E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.18604651162790728</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.11627906976744162</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.38372093023255804</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.30232558139534887</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'51.8 cm'!$C$6:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>443.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-72E9-4FE6-99E1-9703A63D013E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Paracord</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'51.8 cm'!$N$6:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'51.8 cm'!$K$6:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-72E9-4FE6-99E1-9703A63D013E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Brake Cable</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'51.8 cm'!$N$23:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'51.8 cm'!$K$23:$K$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-72E9-4FE6-99E1-9703A63D013E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="406590880"/>
+        <c:axId val="406592960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="406590880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406592960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="406592960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406590880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2750,6 +3365,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4815,6 +5470,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5497,16 +6668,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5514,6 +6685,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{982C00CA-6616-41F5-A4BF-4F315A7F5C2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946073EC-4C02-4769-B522-FFE9F4DD1189}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6039,7 +7253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -7125,11 +8339,11 @@
         <v>620</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E24" si="0">1-A7/$B$1</f>
+        <f t="shared" ref="E7:E23" si="0">1-A7/$B$1</f>
         <v>0.15164835164835166</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F24" si="1">E7/$B$3</f>
+        <f t="shared" ref="F7:F23" si="1">E7/$B$3</f>
         <v>0.95833333333333348</v>
       </c>
     </row>
@@ -7265,7 +8479,7 @@
         <v>58.9</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C24" si="2">B14*4.4482216</f>
+        <f t="shared" ref="C14:C23" si="2">B14*4.4482216</f>
         <v>262.00025224000001</v>
       </c>
       <c r="D14">
@@ -7546,8 +8760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C902C6E6-059B-43BE-A924-BB7C80CB41D4}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8096,4 +9310,569 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2BFFE4-73AB-4B28-8B60-9C656B1F81F0}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>518</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>432</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>1-B2/B1</f>
+        <v>0.16602316602316602</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>432</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>619</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E26" si="0">1-A6/$B$1</f>
+        <v>0.16602316602316602</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F26" si="1">E6/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>431</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>618</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.16795366795366795</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1.0116279069767442</v>
+      </c>
+      <c r="G7">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>429</v>
+      </c>
+      <c r="C8">
+        <v>-5.3</v>
+      </c>
+      <c r="D8">
+        <v>618</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.1718146718146718</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.0348837209302324</v>
+      </c>
+      <c r="G8">
+        <v>663</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>440</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>616</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.15057915057915061</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.90697674418604668</v>
+      </c>
+      <c r="G9">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>515</v>
+      </c>
+      <c r="C10">
+        <v>443.2</v>
+      </c>
+      <c r="D10">
+        <v>615</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>5.7915057915057799E-3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3.4883720930232488E-2</v>
+      </c>
+      <c r="G10">
+        <v>755</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>506</v>
+      </c>
+      <c r="C11">
+        <v>347</v>
+      </c>
+      <c r="D11">
+        <v>616.79999999999995</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.316602316602312E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.13953488372092995</v>
+      </c>
+      <c r="G11">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>498</v>
+      </c>
+      <c r="C12">
+        <v>296</v>
+      </c>
+      <c r="D12">
+        <v>618</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3.8610038610038644E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.23255813953488391</v>
+      </c>
+      <c r="G12">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>489</v>
+      </c>
+      <c r="C13">
+        <v>245</v>
+      </c>
+      <c r="D13">
+        <v>617</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>5.5984555984555984E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.33720930232558138</v>
+      </c>
+      <c r="G13">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>477</v>
+      </c>
+      <c r="C14">
+        <v>191</v>
+      </c>
+      <c r="D14">
+        <v>617</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>7.9150579150579103E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.47674418604651136</v>
+      </c>
+      <c r="G14">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>439</v>
+      </c>
+      <c r="C15">
+        <v>55</v>
+      </c>
+      <c r="D15">
+        <v>617</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.15250965250965254</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.91860465116279089</v>
+      </c>
+      <c r="G15">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>448</v>
+      </c>
+      <c r="C16">
+        <v>99</v>
+      </c>
+      <c r="D16">
+        <v>617</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.13513513513513509</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.81395348837209269</v>
+      </c>
+      <c r="G16">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>458</v>
+      </c>
+      <c r="C17">
+        <v>132</v>
+      </c>
+      <c r="D17">
+        <v>617</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.11583011583011582</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.69767441860465107</v>
+      </c>
+      <c r="G17">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>465</v>
+      </c>
+      <c r="C18">
+        <v>160</v>
+      </c>
+      <c r="D18">
+        <v>617</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.10231660231660233</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.61627906976744196</v>
+      </c>
+      <c r="G18">
+        <v>703</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>473</v>
+      </c>
+      <c r="C19">
+        <v>195</v>
+      </c>
+      <c r="D19">
+        <v>617</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>8.6872586872586921E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.52325581395348864</v>
+      </c>
+      <c r="G19">
+        <v>711</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>516</v>
+      </c>
+      <c r="C20">
+        <v>450</v>
+      </c>
+      <c r="D20">
+        <v>617</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>3.8610038610038533E-3</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2.3255813953488327E-2</v>
+      </c>
+      <c r="G20">
+        <v>755</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>512</v>
+      </c>
+      <c r="C21">
+        <v>420</v>
+      </c>
+      <c r="D21">
+        <v>617</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.158301158301156E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>6.9767441860464977E-2</v>
+      </c>
+      <c r="G21">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>502</v>
+      </c>
+      <c r="C22">
+        <v>328</v>
+      </c>
+      <c r="D22">
+        <v>617</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>3.0888030888030937E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0.18604651162790728</v>
+      </c>
+      <c r="G22">
+        <v>742</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>508</v>
+      </c>
+      <c r="C23">
+        <v>378</v>
+      </c>
+      <c r="D23">
+        <v>617</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.9305019305019266E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.11627906976744162</v>
+      </c>
+      <c r="G23">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>485</v>
+      </c>
+      <c r="C24">
+        <v>230</v>
+      </c>
+      <c r="D24">
+        <v>617</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>6.370656370656369E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0.38372093023255804</v>
+      </c>
+      <c r="G24">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>492</v>
+      </c>
+      <c r="C25">
+        <v>278</v>
+      </c>
+      <c r="D25">
+        <v>617</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>5.0193050193050204E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0.30232558139534887</v>
+      </c>
+      <c r="G25">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>518</v>
+      </c>
+      <c r="C26">
+        <v>518</v>
+      </c>
+      <c r="D26">
+        <v>617</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>761</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added one more length
Added one more length of BPA for max force measurement. Very short. Helps find the zero value for the max force equation.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF11DBC0-7303-43C8-966F-40BD2E875E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E898D191-3362-4FEB-A6F0-A15376E5A468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="49">
   <si>
     <t>Force (lbs)</t>
   </si>
@@ -3615,10 +3615,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$3:$W$3</c:f>
+              <c:f>'Fmax(L)'!$C$3:$X$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>845</c:v>
                 </c:pt>
@@ -3681,16 +3681,19 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$6:$W$6</c:f>
+              <c:f>'Fmax(L)'!$C$6:$X$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>447.1</c:v>
                 </c:pt>
@@ -3753,6 +3756,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>396.17</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.3000000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4017,10 +4023,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$3:$W$3</c:f>
+              <c:f>'Fmax(L)'!$C$3:$X$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>845</c:v>
                 </c:pt>
@@ -4083,16 +4089,19 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$5:$W$5</c:f>
+              <c:f>'Fmax(L)'!$C$5:$X$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0.17159763313609466</c:v>
                 </c:pt>
@@ -4155,6 +4164,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.16580310880829019</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.9999999999999978E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11152,8 +11164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CFFEA6-F038-4ADE-B4DB-050B0246E0CF}">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11219,6 +11231,9 @@
       <c r="W1" s="21">
         <v>12</v>
       </c>
+      <c r="X1" s="21">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
@@ -11256,10 +11271,27 @@
       <c r="Q2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
+      <c r="R2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -11327,6 +11359,9 @@
       </c>
       <c r="W3" s="20">
         <v>193</v>
+      </c>
+      <c r="X3" s="20">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -11386,6 +11421,9 @@
       <c r="W4" s="20">
         <v>161</v>
       </c>
+      <c r="X4" s="20">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -11470,6 +11508,10 @@
         <f t="shared" si="2"/>
         <v>0.16580310880829019</v>
       </c>
+      <c r="X5" s="19">
+        <f t="shared" ref="X5" si="3">1-X4/X3</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -11538,6 +11580,9 @@
       <c r="W6" s="20">
         <v>396.17</v>
       </c>
+      <c r="X6" s="20">
+        <v>8.3000000000000007</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -11604,6 +11649,9 @@
         <v>48</v>
       </c>
       <c r="W7" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -11707,11 +11755,11 @@
         <v>200</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" ref="G10:G14" si="3">1-B10/$D$3</f>
+        <f t="shared" ref="G10:G14" si="4">1-B10/$D$3</f>
         <v>2.3809523809523725E-3</v>
       </c>
       <c r="H10" s="12">
-        <f t="shared" ref="H10:H14" si="4">G10/$D$5</f>
+        <f t="shared" ref="H10:H14" si="5">G10/$D$5</f>
         <v>1.3793103448275808E-2</v>
       </c>
       <c r="L10" t="s">
@@ -11734,11 +11782,11 @@
         <v>300</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.5714285714285587E-3</v>
       </c>
       <c r="H11" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.0689655172413713E-2</v>
       </c>
     </row>
@@ -11758,11 +11806,11 @@
         <v>400</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.761904761904745E-3</v>
       </c>
       <c r="H12" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7586206896551616E-2</v>
       </c>
     </row>
@@ -11782,11 +11830,11 @@
         <v>500</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9523809523809312E-3</v>
       </c>
       <c r="H13" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689523E-2</v>
       </c>
     </row>
@@ -11806,11 +11854,11 @@
         <v>620</v>
       </c>
       <c r="G14" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.1428571428571175E-3</v>
       </c>
       <c r="H14" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.1379310344827426E-2</v>
       </c>
       <c r="X14" t="s">
@@ -11874,11 +11922,11 @@
         <v>200</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" ref="G16:G20" si="5">1-B16/$F$3</f>
+        <f t="shared" ref="G16:G20" si="6">1-B16/$F$3</f>
         <v>0</v>
       </c>
       <c r="H16" s="7">
-        <f t="shared" ref="H16:H20" si="6">G16/$F$5</f>
+        <f t="shared" ref="H16:H20" si="7">G16/$F$5</f>
         <v>0</v>
       </c>
       <c r="X16">
@@ -11907,11 +11955,11 @@
         <v>300</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.2820512820512775E-3</v>
       </c>
       <c r="H17" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.5187969924811783E-3</v>
       </c>
       <c r="X17">
@@ -11940,11 +11988,11 @@
         <v>400</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X18">
@@ -11973,11 +12021,11 @@
         <v>500</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H19" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X19">
@@ -12006,11 +12054,11 @@
         <v>620</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K20" s="1"/>
@@ -12060,11 +12108,11 @@
         <v>200</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" ref="G22:G26" si="7">1-B22/$H$3</f>
+        <f t="shared" ref="G22:G26" si="8">1-B22/$H$3</f>
         <v>0</v>
       </c>
       <c r="H22" s="7">
-        <f t="shared" ref="H22:H38" si="8">G22/$H$5</f>
+        <f t="shared" ref="H22:H32" si="9">G22/$H$5</f>
         <v>0</v>
       </c>
     </row>
@@ -12084,11 +12132,11 @@
         <v>300</v>
       </c>
       <c r="G23" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4104372355430161E-3</v>
       </c>
       <c r="H23" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.0645161290322474E-3</v>
       </c>
       <c r="K23" s="1"/>
@@ -12117,11 +12165,11 @@
         <v>400</v>
       </c>
       <c r="G24" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4104372355430161E-3</v>
       </c>
       <c r="H24" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.0645161290322474E-3</v>
       </c>
     </row>
@@ -12141,11 +12189,11 @@
         <v>500</v>
       </c>
       <c r="G25" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.8208744710860323E-3</v>
       </c>
       <c r="H25" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6129032258064495E-2</v>
       </c>
     </row>
@@ -12165,11 +12213,11 @@
         <v>620</v>
       </c>
       <c r="G26" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.8208744710860323E-3</v>
       </c>
       <c r="H26" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6129032258064495E-2</v>
       </c>
     </row>
@@ -12215,11 +12263,11 @@
         <v>200</v>
       </c>
       <c r="G28" s="6">
-        <f t="shared" ref="G28:G32" si="9">1-B28/$J$3</f>
+        <f t="shared" ref="G28:G32" si="10">1-B28/$J$3</f>
         <v>0</v>
       </c>
       <c r="H28" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12239,11 +12287,11 @@
         <v>300</v>
       </c>
       <c r="G29" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="7">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="7">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -12263,11 +12311,11 @@
         <v>400</v>
       </c>
       <c r="G30" s="6">
+        <f t="shared" si="10"/>
+        <v>1.7513134851138146E-3</v>
+      </c>
+      <c r="H30" s="7">
         <f t="shared" si="9"/>
-        <v>1.7513134851138146E-3</v>
-      </c>
-      <c r="H30" s="7">
-        <f t="shared" si="8"/>
         <v>1.0013558556013668E-2</v>
       </c>
     </row>
@@ -12287,11 +12335,11 @@
         <v>500</v>
       </c>
       <c r="G31" s="6">
+        <f t="shared" si="10"/>
+        <v>1.7513134851138146E-3</v>
+      </c>
+      <c r="H31" s="7">
         <f t="shared" si="9"/>
-        <v>1.7513134851138146E-3</v>
-      </c>
-      <c r="H31" s="7">
-        <f t="shared" si="8"/>
         <v>1.0013558556013668E-2</v>
       </c>
     </row>
@@ -12311,11 +12359,11 @@
         <v>620</v>
       </c>
       <c r="G32" s="9">
+        <f t="shared" si="10"/>
+        <v>1.7513134851138146E-3</v>
+      </c>
+      <c r="H32" s="10">
         <f t="shared" si="9"/>
-        <v>1.7513134851138146E-3</v>
-      </c>
-      <c r="H32" s="10">
-        <f t="shared" si="8"/>
         <v>1.0013558556013668E-2</v>
       </c>
     </row>
@@ -12364,11 +12412,11 @@
         <v>200</v>
       </c>
       <c r="G34" s="6">
-        <f t="shared" ref="G34:G38" si="10">1-B34/$P$3</f>
+        <f t="shared" ref="G34:G38" si="11">1-B34/$P$3</f>
         <v>0</v>
       </c>
       <c r="H34" s="7">
-        <f t="shared" ref="H34:H44" si="11">G34/$P$5</f>
+        <f t="shared" ref="H34:H38" si="12">G34/$P$5</f>
         <v>0</v>
       </c>
     </row>
@@ -12388,11 +12436,11 @@
         <v>300</v>
       </c>
       <c r="G35" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H35" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -12412,11 +12460,11 @@
         <v>400</v>
       </c>
       <c r="G36" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.8148820326678861E-3</v>
       </c>
       <c r="H36" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.041666666666672E-2</v>
       </c>
     </row>
@@ -12436,11 +12484,11 @@
         <v>500</v>
       </c>
       <c r="G37" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.8148820326678861E-3</v>
       </c>
       <c r="H37" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.041666666666672E-2</v>
       </c>
     </row>
@@ -12460,11 +12508,11 @@
         <v>620</v>
       </c>
       <c r="G38" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.6297640653357721E-3</v>
       </c>
       <c r="H38" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.083333333333344E-2</v>
       </c>
     </row>
@@ -12513,11 +12561,11 @@
         <v>200</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" ref="G40:G44" si="12">1-B40/$Q$3</f>
+        <f t="shared" ref="G40:G44" si="13">1-B40/$Q$3</f>
         <v>0</v>
       </c>
       <c r="H40" s="7">
-        <f t="shared" ref="H40:H50" si="13">G40/$Q$5</f>
+        <f t="shared" ref="H40:H44" si="14">G40/$Q$5</f>
         <v>0</v>
       </c>
     </row>
@@ -12537,11 +12585,11 @@
         <v>300</v>
       </c>
       <c r="G41" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H41" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -12561,11 +12609,11 @@
         <v>400</v>
       </c>
       <c r="G42" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -12585,11 +12633,11 @@
         <v>500</v>
       </c>
       <c r="G43" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H43" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -12609,11 +12657,11 @@
         <v>620</v>
       </c>
       <c r="G44" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.7700831024930483E-3</v>
       </c>
       <c r="H44" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.612903225806436E-2</v>
       </c>
     </row>
@@ -12662,11 +12710,11 @@
         <v>200</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" ref="G46:G51" si="14">1-B46/$R$3</f>
+        <f t="shared" ref="G46:G50" si="15">1-B46/$R$3</f>
         <v>0</v>
       </c>
       <c r="H46" s="7">
-        <f t="shared" ref="H46:H51" si="15">G46/$R$5</f>
+        <f t="shared" ref="H46:H50" si="16">G46/$R$5</f>
         <v>0</v>
       </c>
     </row>
@@ -12686,11 +12734,11 @@
         <v>300</v>
       </c>
       <c r="G47" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H47" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -12710,11 +12758,11 @@
         <v>400</v>
       </c>
       <c r="G48" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H48" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -12734,11 +12782,11 @@
         <v>500</v>
       </c>
       <c r="G49" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H49" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -12758,11 +12806,11 @@
         <v>620</v>
       </c>
       <c r="G50" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H50" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -12811,11 +12859,11 @@
         <v>620</v>
       </c>
       <c r="G52" s="25">
-        <f t="shared" ref="G52:G58" si="16">1-B52/$S$3</f>
+        <f t="shared" ref="G52:G54" si="17">1-B52/$S$3</f>
         <v>0</v>
       </c>
       <c r="H52" s="26">
-        <f t="shared" ref="H52:H58" si="17">G52/$S$5</f>
+        <f t="shared" ref="H52:H54" si="18">G52/$S$5</f>
         <v>0</v>
       </c>
     </row>
@@ -12864,11 +12912,11 @@
         <v>620</v>
       </c>
       <c r="G54" s="25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-1.2592592592592591</v>
       </c>
       <c r="H54" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-8.5</v>
       </c>
     </row>
@@ -13031,25 +13079,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
+        <v>13</v>
+      </c>
+      <c r="B61" s="4">
+        <v>10</v>
+      </c>
       <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="24"/>
+      <c r="D61" s="4">
+        <v>0</v>
+      </c>
+      <c r="E61" s="4">
+        <v>0</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0</v>
+      </c>
+      <c r="G61" s="25">
+        <f>1-B61/$X$3</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="26">
+        <f>G61/$X$5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
-      <c r="B62" s="9"/>
+      <c r="B62" s="9">
+        <v>10</v>
+      </c>
       <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="26"/>
+      <c r="D62" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E62" s="9">
+        <v>620</v>
+      </c>
+      <c r="F62" s="9">
+        <v>620</v>
+      </c>
+      <c r="G62" s="25">
+        <f>1-B62/$X$3</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="26">
+        <f>G62/$X$5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>

</xml_diff>

<commit_message>
added lawrence's Fmax and kmax data
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06D40AA-B3B9-43A9-950E-084EC9204F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC0CD3-E70C-43D7-B1DE-E62A2704BE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="49">
   <si>
     <t>Force (lbs)</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>*11.23 N pretension, 320 N measured</t>
+  </si>
+  <si>
+    <t>Lawrence's Tests</t>
   </si>
 </sst>
 </file>
@@ -3763,10 +3766,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$3:$X$3</c:f>
+              <c:f>'Fmax(L)'!$C$3:$AC$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>845</c:v>
                 </c:pt>
@@ -3832,16 +3835,31 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$6:$X$6</c:f>
+              <c:f>'Fmax(L)'!$C$6:$AC$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>447.1</c:v>
                 </c:pt>
@@ -3907,6 +3925,21 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>343.05</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>377.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>377.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>418.19</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>402.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4169,12 +4202,27 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.1962965638469504E-2"/>
+                  <c:y val="0.2927223097112861"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$3:$X$3</c:f>
+              <c:f>'Fmax(L)'!$C$3:$AC$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>845</c:v>
                 </c:pt>
@@ -4240,16 +4288,31 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$5:$X$5</c:f>
+              <c:f>'Fmax(L)'!$C$5:$AC$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>0.17159763313609466</c:v>
                 </c:pt>
@@ -4315,6 +4378,21 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>9.9999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.15909090909090906</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.16153846153846152</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.16370106761565839</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.14590747330960852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10718,7 +10796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2BFFE4-73AB-4B28-8B60-9C656B1F81F0}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -11299,10 +11377,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CFFEA6-F038-4ADE-B4DB-050B0246E0CF}">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11317,7 +11395,7 @@
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
@@ -11369,10 +11447,13 @@
         <v>12</v>
       </c>
       <c r="X1" s="21">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>32</v>
       </c>
@@ -11430,7 +11511,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -11500,8 +11581,23 @@
       <c r="X3" s="20">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y3" s="20">
+        <v>120</v>
+      </c>
+      <c r="Z3" s="20">
+        <v>220</v>
+      </c>
+      <c r="AA3" s="20">
+        <v>260</v>
+      </c>
+      <c r="AB3" s="20">
+        <v>281</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -11561,8 +11657,23 @@
       <c r="X4" s="20">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y4" s="20">
+        <v>100</v>
+      </c>
+      <c r="Z4" s="20">
+        <v>185</v>
+      </c>
+      <c r="AA4" s="20">
+        <v>218</v>
+      </c>
+      <c r="AB4" s="20">
+        <v>235</v>
+      </c>
+      <c r="AC4" s="20">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -11646,11 +11757,31 @@
         <v>0.16580310880829019</v>
       </c>
       <c r="X5" s="19">
-        <f t="shared" ref="X5" si="3">1-X4/X3</f>
+        <f t="shared" ref="X5:AC5" si="3">1-X4/X3</f>
         <v>9.9999999999999978E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y5" s="19">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="Z5" s="19">
+        <f t="shared" si="3"/>
+        <v>0.15909090909090906</v>
+      </c>
+      <c r="AA5" s="19">
+        <f t="shared" si="3"/>
+        <v>0.16153846153846152</v>
+      </c>
+      <c r="AB5" s="19">
+        <f t="shared" si="3"/>
+        <v>0.16370106761565839</v>
+      </c>
+      <c r="AC5" s="19">
+        <f t="shared" si="3"/>
+        <v>0.14590747330960852</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
@@ -11720,8 +11851,23 @@
       <c r="X6" s="20">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y6" s="20">
+        <v>343.05</v>
+      </c>
+      <c r="Z6" s="20">
+        <v>377.2</v>
+      </c>
+      <c r="AA6" s="20">
+        <v>377.2</v>
+      </c>
+      <c r="AB6" s="20">
+        <v>418.19</v>
+      </c>
+      <c r="AC6" s="20">
+        <v>402.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
@@ -11791,8 +11937,20 @@
       <c r="X7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -11840,7 +11998,7 @@
       </c>
       <c r="S8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -11876,7 +12034,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6">
         <v>838</v>
@@ -11903,7 +12061,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6">
         <v>837</v>
@@ -11927,7 +12085,7 @@
         <v>2.0689655172413713E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6">
         <v>836</v>
@@ -11951,7 +12109,7 @@
         <v>2.7586206896551616E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6">
         <v>835</v>
@@ -11975,7 +12133,7 @@
         <v>3.4482758620689523E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="9">
         <v>834</v>
@@ -12008,7 +12166,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -12043,7 +12201,7 @@
         <v>0.1607142857142857</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="11">
         <v>780</v>

</xml_diff>

<commit_message>
Improved fit. Max. force function is good to go.
Maximum force at max pressure as a function of resting length is good. Maximum force as a function of resting length and pressure is really good. Hypothesis that max strain is a linear or quadratic function of resting length is disproven.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC0CD3-E70C-43D7-B1DE-E62A2704BE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0252ED3-4FAC-4CA4-A94F-B6859B66C890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="50">
   <si>
     <t>Force (lbs)</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Muscle</t>
   </si>
   <si>
-    <t>pressure (set)</t>
-  </si>
-  <si>
-    <t>Force</t>
-  </si>
-  <si>
     <t>Pressure measured (kPa)</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
   </si>
   <si>
     <t>vertical</t>
-  </si>
-  <si>
-    <t>Len</t>
   </si>
   <si>
     <t>Resting L</t>
@@ -186,6 +177,18 @@
   <si>
     <t>Lawrence's Tests</t>
   </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>FORCE</t>
+  </si>
+  <si>
+    <t>PRESSURE</t>
+  </si>
 </sst>
 </file>
 
@@ -222,7 +225,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -367,11 +370,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -403,6 +443,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8529,7 +8573,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8545,10 +8589,10 @@
         <v>112</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -8759,10 +8803,10 @@
         <v>415</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -9754,10 +9798,10 @@
         <v>455</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1"/>
       <c r="M1" s="1"/>
@@ -10233,7 +10277,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10254,10 +10298,10 @@
         <v>490</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1"/>
       <c r="M1" s="1"/>
@@ -10392,7 +10436,7 @@
         <v>737</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -10418,7 +10462,7 @@
         <v>724</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -10818,10 +10862,10 @@
         <v>518</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1"/>
       <c r="M1" s="1"/>
@@ -10983,7 +11027,7 @@
         <v>755</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -11353,7 +11397,7 @@
         <v>761</v>
       </c>
       <c r="H26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -11379,8 +11423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CFFEA6-F038-4ADE-B4DB-050B0246E0CF}">
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:AC6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X41" sqref="X41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11416,7 +11460,7 @@
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -11450,33 +11494,33 @@
         <v>13</v>
       </c>
       <c r="Y1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="6"/>
@@ -11484,31 +11528,31 @@
       <c r="N2" s="6"/>
       <c r="O2" s="7"/>
       <c r="P2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="X2" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -11783,7 +11827,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="16">
         <v>447.1</v>
@@ -11869,85 +11913,85 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" t="s">
+        <v>38</v>
+      </c>
+      <c r="V7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" t="s">
-        <v>41</v>
-      </c>
-      <c r="S7" t="s">
-        <v>41</v>
-      </c>
-      <c r="T7" t="s">
-        <v>41</v>
-      </c>
-      <c r="U7" t="s">
-        <v>41</v>
-      </c>
-      <c r="V7" t="s">
-        <v>43</v>
-      </c>
       <c r="W7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="X7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="Y7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Z7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AA7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AB7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:29" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11964,10 +12008,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>2</v>
@@ -11975,27 +12019,13 @@
       <c r="H8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>200</v>
-      </c>
-      <c r="O8">
-        <v>300</v>
-      </c>
-      <c r="P8">
-        <v>400</v>
-      </c>
-      <c r="Q8">
-        <v>500</v>
-      </c>
-      <c r="R8">
-        <v>620</v>
-      </c>
+      <c r="L8" s="2"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
       <c r="S8"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
@@ -12022,9 +12052,6 @@
       <c r="H9" s="12">
         <f>G9/$D$5</f>
         <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>29</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -12057,9 +12084,6 @@
         <f t="shared" ref="H10:H14" si="5">G10/$D$5</f>
         <v>1.3793103448275808E-2</v>
       </c>
-      <c r="L10" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -12157,13 +12181,13 @@
         <v>4.1379310344827426E-2</v>
       </c>
       <c r="X14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Y14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Z14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -12566,7 +12590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="11">
         <v>571</v>
@@ -12589,8 +12613,17 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="11">
         <v>570</v>
@@ -12612,6 +12645,33 @@
       <c r="H30" s="7">
         <f t="shared" si="9"/>
         <v>1.0013558556013668E-2</v>
+      </c>
+      <c r="L30" t="s">
+        <v>47</v>
+      </c>
+      <c r="M30" s="27">
+        <v>0</v>
+      </c>
+      <c r="N30" s="28">
+        <v>100</v>
+      </c>
+      <c r="O30" s="28">
+        <v>200</v>
+      </c>
+      <c r="P30" s="28">
+        <v>300</v>
+      </c>
+      <c r="Q30" s="28">
+        <v>400</v>
+      </c>
+      <c r="R30" s="28">
+        <v>500</v>
+      </c>
+      <c r="S30" s="28">
+        <v>620</v>
+      </c>
+      <c r="T30" s="30" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -12637,6 +12697,33 @@
         <f t="shared" si="9"/>
         <v>1.0013558556013668E-2</v>
       </c>
+      <c r="L31" s="17">
+        <v>840</v>
+      </c>
+      <c r="M31" s="6">
+        <v>0</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O31" s="6">
+        <v>114.32</v>
+      </c>
+      <c r="P31" s="6">
+        <v>191.8</v>
+      </c>
+      <c r="Q31" s="11">
+        <v>275.2</v>
+      </c>
+      <c r="R31" s="11">
+        <v>355.4</v>
+      </c>
+      <c r="S31" s="7">
+        <v>447.1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
@@ -12661,8 +12748,35 @@
         <f t="shared" si="9"/>
         <v>1.0013558556013668E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L32" s="18">
+        <v>780</v>
+      </c>
+      <c r="M32" s="6">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O32" s="11">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="P32" s="11">
+        <v>216</v>
+      </c>
+      <c r="Q32" s="11">
+        <v>299.7</v>
+      </c>
+      <c r="R32" s="11">
+        <v>378.1</v>
+      </c>
+      <c r="S32" s="7">
+        <v>472</v>
+      </c>
+      <c r="U32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>5</v>
       </c>
@@ -12688,10 +12802,37 @@
         <v>-1.0416666666666083E-2</v>
       </c>
       <c r="I33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="L33" s="18">
+        <v>709</v>
+      </c>
+      <c r="M33" s="6">
+        <v>0</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O33" s="11">
+        <v>124.21</v>
+      </c>
+      <c r="P33" s="11">
+        <v>201.4</v>
+      </c>
+      <c r="Q33" s="11">
+        <v>276.02</v>
+      </c>
+      <c r="R33" s="11">
+        <v>355.9</v>
+      </c>
+      <c r="S33" s="7">
+        <v>452.32</v>
+      </c>
+      <c r="U33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="11">
         <v>551</v>
@@ -12714,8 +12855,35 @@
         <f t="shared" ref="H34:H38" si="12">G34/$P$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L34" s="18">
+        <v>571</v>
+      </c>
+      <c r="M34" s="6">
+        <v>0</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O34" s="11">
+        <v>136.1</v>
+      </c>
+      <c r="P34" s="11">
+        <v>212.39</v>
+      </c>
+      <c r="Q34" s="11">
+        <v>288.2</v>
+      </c>
+      <c r="R34" s="11">
+        <v>366.94</v>
+      </c>
+      <c r="S34" s="7">
+        <v>461.6</v>
+      </c>
+      <c r="U34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="11">
         <v>551</v>
@@ -12738,8 +12906,35 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L35" s="18">
+        <v>112</v>
+      </c>
+      <c r="M35" s="6">
+        <v>0</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S35" s="22">
+        <v>334</v>
+      </c>
+      <c r="U35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="11">
         <v>550</v>
@@ -12762,8 +12957,35 @@
         <f t="shared" si="12"/>
         <v>1.041666666666672E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L36" s="18">
+        <v>415</v>
+      </c>
+      <c r="M36" s="6">
+        <v>0</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S36" s="22">
+        <v>444.8</v>
+      </c>
+      <c r="U36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="11">
         <v>550</v>
@@ -12786,8 +13008,35 @@
         <f t="shared" si="12"/>
         <v>1.041666666666672E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L37" s="18">
+        <v>455</v>
+      </c>
+      <c r="M37" s="6">
+        <v>0</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S37" s="22">
+        <v>460</v>
+      </c>
+      <c r="U37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="9">
         <v>549</v>
@@ -12810,8 +13059,35 @@
         <f t="shared" si="12"/>
         <v>2.083333333333344E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L38" s="18">
+        <v>490</v>
+      </c>
+      <c r="M38" s="6">
+        <v>0</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S38" s="22">
+        <v>451.38</v>
+      </c>
+      <c r="U38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>6</v>
       </c>
@@ -12837,10 +13113,37 @@
         <v>-1.612903225806436E-2</v>
       </c>
       <c r="I39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="L39" s="18">
+        <v>518</v>
+      </c>
+      <c r="M39" s="6">
+        <v>0</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S39" s="22">
+        <v>455.83</v>
+      </c>
+      <c r="U39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="11">
         <v>361</v>
@@ -12863,8 +13166,35 @@
         <f t="shared" ref="H40:H44" si="14">G40/$Q$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L40" s="18">
+        <v>551</v>
+      </c>
+      <c r="M40" s="6">
+        <v>0</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O40" s="11">
+        <v>129.26</v>
+      </c>
+      <c r="P40" s="11">
+        <v>201.3</v>
+      </c>
+      <c r="Q40" s="11">
+        <v>282.33999999999997</v>
+      </c>
+      <c r="R40" s="11">
+        <v>360.24</v>
+      </c>
+      <c r="S40" s="7">
+        <v>453.14</v>
+      </c>
+      <c r="U40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="11">
         <v>361</v>
@@ -12887,8 +13217,35 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L41" s="18">
+        <v>361</v>
+      </c>
+      <c r="M41" s="6">
+        <v>0</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O41" s="11">
+        <v>121.5</v>
+      </c>
+      <c r="P41" s="11">
+        <v>192.91</v>
+      </c>
+      <c r="Q41" s="11">
+        <v>269</v>
+      </c>
+      <c r="R41" s="11">
+        <v>344.5</v>
+      </c>
+      <c r="S41" s="7">
+        <v>436.4</v>
+      </c>
+      <c r="U41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="11">
         <v>361</v>
@@ -12911,8 +13268,35 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L42" s="20">
+        <v>54</v>
+      </c>
+      <c r="M42" s="6">
+        <v>0</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O42" s="11">
+        <v>56.1</v>
+      </c>
+      <c r="P42" s="11">
+        <v>103.37</v>
+      </c>
+      <c r="Q42" s="11">
+        <v>155.44999999999999</v>
+      </c>
+      <c r="R42" s="11">
+        <v>207</v>
+      </c>
+      <c r="S42" s="7">
+        <v>266.5</v>
+      </c>
+      <c r="U42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="11">
         <v>361</v>
@@ -12935,8 +13319,35 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L43" s="20">
+        <v>27</v>
+      </c>
+      <c r="M43" s="6">
+        <v>0</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S43" s="22">
+        <v>135.32</v>
+      </c>
+      <c r="U43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="9">
         <v>360</v>
@@ -12959,8 +13370,35 @@
         <f t="shared" si="14"/>
         <v>1.612903225806436E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L44" s="20">
+        <v>69</v>
+      </c>
+      <c r="M44" s="6">
+        <v>0</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S44" s="22">
+        <v>271.48</v>
+      </c>
+      <c r="U44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>7</v>
       </c>
@@ -12986,10 +13424,37 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="L45" s="20">
+        <v>275</v>
+      </c>
+      <c r="M45" s="6">
+        <v>0</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S45" s="22">
+        <v>412.3</v>
+      </c>
+      <c r="U45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="11">
         <v>54</v>
@@ -13012,8 +13477,35 @@
         <f t="shared" ref="H46:H50" si="16">G46/$R$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L46" s="20">
+        <v>151</v>
+      </c>
+      <c r="M46" s="6">
+        <v>0</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R46" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S46" s="22">
+        <v>347.11</v>
+      </c>
+      <c r="U46">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="11">
         <v>54</v>
@@ -13036,8 +13528,35 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L47" s="20">
+        <v>193</v>
+      </c>
+      <c r="M47" s="6">
+        <v>0</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S47" s="22">
+        <v>396.17</v>
+      </c>
+      <c r="U47">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="11">
         <v>54</v>
@@ -13060,8 +13579,35 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L48" s="20">
+        <v>10</v>
+      </c>
+      <c r="M48" s="6">
+        <v>0</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O48" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P48" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R48" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S48" s="22">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="U48">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="11">
         <v>54</v>
@@ -13084,8 +13630,35 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L49" s="20">
+        <v>120</v>
+      </c>
+      <c r="M49" s="6">
+        <v>0</v>
+      </c>
+      <c r="N49" s="6">
+        <v>19.7</v>
+      </c>
+      <c r="O49" s="6">
+        <v>66</v>
+      </c>
+      <c r="P49" s="6">
+        <v>124.82</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>195.1</v>
+      </c>
+      <c r="R49" s="6">
+        <v>258.3</v>
+      </c>
+      <c r="S49" s="22">
+        <v>341.5</v>
+      </c>
+      <c r="U49">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="9">
         <v>54</v>
@@ -13108,8 +13681,35 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L50" s="20">
+        <v>220</v>
+      </c>
+      <c r="M50" s="6">
+        <v>0</v>
+      </c>
+      <c r="N50" s="6">
+        <v>23</v>
+      </c>
+      <c r="O50" s="6">
+        <v>80.8</v>
+      </c>
+      <c r="P50" s="6">
+        <v>146.19999999999999</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>215.6</v>
+      </c>
+      <c r="R50" s="6">
+        <v>289.8</v>
+      </c>
+      <c r="S50" s="22">
+        <v>377.23</v>
+      </c>
+      <c r="U50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>8</v>
       </c>
@@ -13135,10 +13735,37 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="L51" s="18">
+        <v>260</v>
+      </c>
+      <c r="M51" s="6">
+        <v>0</v>
+      </c>
+      <c r="N51" s="6">
+        <v>31.9</v>
+      </c>
+      <c r="O51" s="6">
+        <v>89.7</v>
+      </c>
+      <c r="P51" s="6">
+        <v>154.6</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>225.3</v>
+      </c>
+      <c r="R51" s="6">
+        <v>294.8</v>
+      </c>
+      <c r="S51" s="22">
+        <v>385.4</v>
+      </c>
+      <c r="U51">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="9">
         <v>27</v>
@@ -13161,8 +13788,35 @@
         <f t="shared" ref="H52:H54" si="18">G52/$S$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L52" s="18">
+        <v>281</v>
+      </c>
+      <c r="M52" s="6">
+        <v>0</v>
+      </c>
+      <c r="N52" s="6">
+        <v>54.65</v>
+      </c>
+      <c r="O52" s="6">
+        <v>117.8</v>
+      </c>
+      <c r="P52" s="6">
+        <v>185</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>257.2</v>
+      </c>
+      <c r="R52" s="6">
+        <v>329.9</v>
+      </c>
+      <c r="S52" s="22">
+        <v>415.8</v>
+      </c>
+      <c r="U52">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>9</v>
       </c>
@@ -13188,10 +13842,37 @@
         <v>0.72727272727272685</v>
       </c>
       <c r="I53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="L53" s="18">
+        <v>281</v>
+      </c>
+      <c r="M53" s="9">
+        <v>0</v>
+      </c>
+      <c r="N53" s="9">
+        <v>37.1</v>
+      </c>
+      <c r="O53" s="9">
+        <v>101.1</v>
+      </c>
+      <c r="P53" s="9">
+        <v>170.4</v>
+      </c>
+      <c r="Q53" s="9">
+        <v>242.3</v>
+      </c>
+      <c r="R53" s="9">
+        <v>314.2</v>
+      </c>
+      <c r="S53" s="26">
+        <v>406</v>
+      </c>
+      <c r="U53">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
       <c r="B54" s="25">
         <v>61</v>
@@ -13214,8 +13895,14 @@
         <f t="shared" si="18"/>
         <v>-8.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L54" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>10</v>
       </c>
@@ -13241,10 +13928,10 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="9">
         <v>273</v>
@@ -13268,7 +13955,7 @@
         <v>4.2553191489361979E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>11</v>
       </c>
@@ -13294,10 +13981,10 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="9">
         <v>149</v>
@@ -13321,7 +14008,7 @@
         <v>8.6956521739130155E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>12</v>
       </c>
@@ -13347,10 +14034,10 @@
         <v>-3.1250000000000104E-2</v>
       </c>
       <c r="I59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="9">
         <v>193</v>
@@ -13374,7 +14061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>13</v>
       </c>
@@ -13400,7 +14087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="9">
         <v>10</v>
@@ -13424,7 +14111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -13434,7 +14121,7 @@
       <c r="G63" s="23"/>
       <c r="H63" s="24"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>

</xml_diff>

<commit_message>
Finalized 10 and 20 mm normalized force fits
For now
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAFB37B-3D50-44B0-8882-14C128641CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145EDA43-3415-427C-B820-B7BDC2D2567F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -38,6 +38,24 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={C0933719-F29F-4D06-A942-723E036E6640}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C0933719-F29F-4D06-A942-723E036E6640}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changed resting length to 515</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -197,7 +215,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +236,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3154,7 +3178,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Force vs. Relative Strain, 49.0 cm</a:t>
+              <a:t>Force vs. Relative Strain, 51.8 cm</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3290,64 +3314,64 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0116279069767442</c:v>
+                  <c:v>1.0120481927710843</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0348837209302324</c:v>
+                  <c:v>1.0361445783132532</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.90697674418604668</c:v>
+                  <c:v>0.90361445783132577</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4883720930232488E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13953488372092995</c:v>
+                  <c:v>0.10843373493975915</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23255813953488391</c:v>
+                  <c:v>0.20481927710843409</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33720930232558138</c:v>
+                  <c:v>0.31325301204819256</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47674418604651136</c:v>
+                  <c:v>0.45783132530120496</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.91860465116279089</c:v>
+                  <c:v>0.91566265060240992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.81395348837209269</c:v>
+                  <c:v>0.80722891566265076</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.69767441860465107</c:v>
+                  <c:v>0.68674698795180744</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.61627906976744196</c:v>
+                  <c:v>0.6024096385542167</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.52325581395348864</c:v>
+                  <c:v>0.50602409638554247</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3255813953488327E-2</c:v>
+                  <c:v>-1.2048192771084884E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.9767441860464977E-2</c:v>
+                  <c:v>3.6144578313253281E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.18604651162790728</c:v>
+                  <c:v>0.15662650602409661</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.11627906976744162</c:v>
+                  <c:v>8.4337349397590064E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.38372093023255804</c:v>
+                  <c:v>0.36144578313253001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.30232558139534887</c:v>
+                  <c:v>0.27710843373493999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>-3.6144578313253281E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3371,7 +3395,7 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>427.6</c:v>
+                  <c:v>443.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>347</c:v>
@@ -3419,7 +3443,7 @@
                   <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>429</c:v>
+                  <c:v>518</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3922,16 +3946,16 @@
                   <c:v>461.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>334</c:v>
+                  <c:v>348.58</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>444.82220000000001</c:v>
+                  <c:v>459.63</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>451.38</c:v>
+                  <c:v>458.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>455.83</c:v>
@@ -4241,7 +4265,7 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -4387,7 +4411,7 @@
                   <c:v>0.18775510204081636</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16602316602316602</c:v>
+                  <c:v>0.16116504854368929</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.17422867513611617</c:v>
@@ -8266,6 +8290,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ben Bolen" id="{BF8D1625-453C-4F9B-90F4-27D3407028E0}" userId="S::bbolen@pdx.edu::2756ab96-c1b4-4d6e-be6a-ace1ad4a8569" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8561,6 +8591,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2023-12-10T07:41:58.62" personId="{BF8D1625-453C-4F9B-90F4-27D3407028E0}" id="{C0933719-F29F-4D06-A942-723E036E6640}">
+    <text>Changed resting length to 515</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5D9837-CB16-4300-A1DA-BD967A7687F8}">
   <dimension ref="A1:Q14"/>
@@ -8775,8 +8813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9769,8 +9807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050AE67D-A238-4925-A0DE-87F77397D646}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10269,8 +10307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C902C6E6-059B-43BE-A924-BB7C80CB41D4}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10830,11 +10868,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2BFFE4-73AB-4B28-8B60-9C656B1F81F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2BFFE4-73AB-4B28-8B60-9C656B1F81F0}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10852,7 +10890,7 @@
         <v>5</v>
       </c>
       <c r="B1">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D1" t="s">
         <v>37</v>
@@ -10879,7 +10917,7 @@
       </c>
       <c r="B3">
         <f>1-B2/B1</f>
-        <v>0.16602316602316602</v>
+        <v>0.16116504854368929</v>
       </c>
       <c r="I3" s="1"/>
       <c r="M3" s="2"/>
@@ -10919,7 +10957,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E26" si="0">1-A6/$B$1</f>
-        <v>0.16602316602316602</v>
+        <v>0.16116504854368929</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F26" si="1">E6/$B$3</f>
@@ -10941,11 +10979,11 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.16795366795366795</v>
+        <v>0.1631067961165048</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>1.0116279069767442</v>
+        <v>1.0120481927710843</v>
       </c>
       <c r="G7">
         <v>669</v>
@@ -10963,11 +11001,11 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.1718146718146718</v>
+        <v>0.16699029126213594</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>1.0348837209302324</v>
+        <v>1.0361445783132532</v>
       </c>
       <c r="G8">
         <v>663</v>
@@ -10988,11 +11026,11 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.15057915057915061</v>
+        <v>0.14563106796116509</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>0.90697674418604668</v>
+        <v>0.90361445783132577</v>
       </c>
       <c r="G9">
         <v>677</v>
@@ -11003,18 +11041,18 @@
         <v>515</v>
       </c>
       <c r="C10">
-        <v>427.6</v>
+        <v>443.2</v>
       </c>
       <c r="D10">
         <v>615</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>5.7915057915057799E-3</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>3.4883720930232488E-2</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>755</v>
@@ -11035,11 +11073,11 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>2.316602316602312E-2</v>
+        <v>1.747572815533982E-2</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>0.13953488372092995</v>
+        <v>0.10843373493975915</v>
       </c>
       <c r="G11">
         <v>746</v>
@@ -11057,11 +11095,11 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>3.8610038610038644E-2</v>
+        <v>3.300970873786413E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>0.23255813953488391</v>
+        <v>0.20481927710843409</v>
       </c>
       <c r="G12">
         <v>737</v>
@@ -11079,11 +11117,11 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>5.5984555984555984E-2</v>
+        <v>5.0485436893203839E-2</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>0.33720930232558138</v>
+        <v>0.31325301204819256</v>
       </c>
       <c r="G13">
         <v>729</v>
@@ -11101,11 +11139,11 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>7.9150579150579103E-2</v>
+        <v>7.3786407766990303E-2</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0.47674418604651136</v>
+        <v>0.45783132530120496</v>
       </c>
       <c r="G14">
         <v>715</v>
@@ -11123,11 +11161,11 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.15250965250965254</v>
+        <v>0.14757281553398061</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0.91860465116279089</v>
+        <v>0.91566265060240992</v>
       </c>
       <c r="G15">
         <v>675</v>
@@ -11145,11 +11183,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.13513513513513509</v>
+        <v>0.13009708737864079</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0.81395348837209269</v>
+        <v>0.80722891566265076</v>
       </c>
       <c r="G16">
         <v>687</v>
@@ -11167,11 +11205,11 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0.11583011583011582</v>
+        <v>0.11067961165048545</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0.69767441860465107</v>
+        <v>0.68674698795180744</v>
       </c>
       <c r="G17">
         <v>696</v>
@@ -11189,11 +11227,11 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>0.10231660231660233</v>
+        <v>9.7087378640776656E-2</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0.61627906976744196</v>
+        <v>0.6024096385542167</v>
       </c>
       <c r="G18">
         <v>703</v>
@@ -11213,11 +11251,11 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>8.6872586872586921E-2</v>
+        <v>8.1553398058252458E-2</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0.52325581395348864</v>
+        <v>0.50602409638554247</v>
       </c>
       <c r="G19">
         <v>711</v>
@@ -11237,11 +11275,11 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>3.8610038610038533E-3</v>
+        <v>-1.9417475728156219E-3</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>2.3255813953488327E-2</v>
+        <v>-1.2048192771084884E-2</v>
       </c>
       <c r="G20">
         <v>755</v>
@@ -11261,11 +11299,11 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1.158301158301156E-2</v>
+        <v>5.8252427184466438E-3</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>6.9767441860464977E-2</v>
+        <v>3.6144578313253281E-2</v>
       </c>
       <c r="G21">
         <v>753</v>
@@ -11283,11 +11321,11 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>3.0888030888030937E-2</v>
+        <v>2.5242718446601975E-2</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>0.18604651162790728</v>
+        <v>0.15662650602409661</v>
       </c>
       <c r="G22">
         <v>742</v>
@@ -11314,11 +11352,11 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>1.9305019305019266E-2</v>
+        <v>1.3592233009708687E-2</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>0.11627906976744162</v>
+        <v>8.4337349397590064E-2</v>
       </c>
       <c r="G23">
         <v>750</v>
@@ -11336,11 +11374,11 @@
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>6.370656370656369E-2</v>
+        <v>5.8252427184465994E-2</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>0.38372093023255804</v>
+        <v>0.36144578313253001</v>
       </c>
       <c r="G24">
         <v>724</v>
@@ -11358,11 +11396,11 @@
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>5.0193050193050204E-2</v>
+        <v>4.4660194174757306E-2</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>0.30232558139534887</v>
+        <v>0.27710843373493999</v>
       </c>
       <c r="G25">
         <v>734</v>
@@ -11373,18 +11411,18 @@
         <v>518</v>
       </c>
       <c r="C26">
-        <v>429</v>
+        <v>518</v>
       </c>
       <c r="D26">
         <v>617</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5.8252427184466438E-3</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3.6144578313253281E-2</v>
       </c>
       <c r="G26">
         <v>761</v>
@@ -11409,6 +11447,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -11416,8 +11455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CFFEA6-F038-4ADE-B4DB-050B0246E0CF}">
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31:S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11753,7 +11792,7 @@
         <v>0.18775510204081636</v>
       </c>
       <c r="O5" s="9">
-        <v>0.16602316602316602</v>
+        <v>0.16116504854368929</v>
       </c>
       <c r="P5" s="16">
         <f t="shared" ref="P5:W5" si="2">1-P4/P3</f>
@@ -11841,16 +11880,16 @@
         <v>461.6</v>
       </c>
       <c r="K6">
-        <v>334</v>
+        <v>348.58</v>
       </c>
       <c r="L6">
-        <v>444.82220000000001</v>
+        <v>459.63</v>
       </c>
       <c r="M6">
         <v>460</v>
       </c>
       <c r="N6">
-        <v>451.38</v>
+        <v>458.6</v>
       </c>
       <c r="O6">
         <v>455.83</v>
@@ -12891,7 +12930,7 @@
         <v>47</v>
       </c>
       <c r="S35" s="6">
-        <v>334</v>
+        <v>348.58</v>
       </c>
       <c r="U35">
         <v>5</v>
@@ -12941,7 +12980,7 @@
         <v>47</v>
       </c>
       <c r="S36" s="6">
-        <v>444.8</v>
+        <v>459.63</v>
       </c>
       <c r="U36">
         <v>6</v>
@@ -13042,7 +13081,7 @@
         <v>47</v>
       </c>
       <c r="S38" s="6">
-        <v>451.38</v>
+        <v>458.6</v>
       </c>
       <c r="U38">
         <v>8</v>

</xml_diff>

<commit_message>
trying to add 8 more sets of data
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145EDA43-3415-427C-B820-B7BDC2D2567F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42135F9-CA31-48A1-AB31-E7C62C960240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -38,24 +38,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={C0933719-F29F-4D06-A942-723E036E6640}</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C0933719-F29F-4D06-A942-723E036E6640}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Changed resting length to 515</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -215,7 +197,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,12 +218,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -438,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -464,6 +440,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,8 +574,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3314,64 +3291,64 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0120481927710843</c:v>
+                  <c:v>1.0116279069767442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0361445783132532</c:v>
+                  <c:v>1.0348837209302324</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.90361445783132577</c:v>
+                  <c:v>0.90697674418604668</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3.4883720930232488E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13953488372092995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23255813953488391</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33720930232558138</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47674418604651136</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91860465116279089</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.81395348837209269</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.69767441860465107</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.61627906976744196</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.52325581395348864</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3255813953488327E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.9767441860464977E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.18604651162790728</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.11627906976744162</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.38372093023255804</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.30232558139534887</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.10843373493975915</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.20481927710843409</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.31325301204819256</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45783132530120496</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.91566265060240992</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.80722891566265076</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.68674698795180744</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.6024096385542167</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.50602409638554247</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-1.2048192771084884E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.6144578313253281E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.15662650602409661</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.4337349397590064E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.36144578313253001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.27710843373493999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-3.6144578313253281E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3395,7 +3372,7 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>443.2</c:v>
+                  <c:v>427.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>347</c:v>
@@ -3443,7 +3420,7 @@
                   <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>518</c:v>
+                  <c:v>429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3946,10 +3923,10 @@
                   <c:v>461.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>348.58</c:v>
+                  <c:v>334.74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>459.63</c:v>
+                  <c:v>445</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>460</c:v>
@@ -4264,8 +4241,7 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -4280,10 +4256,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$3:$AC$3</c:f>
+              <c:f>'Fmax(L)'!$C$3:$AK$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>845</c:v>
                 </c:pt>
@@ -4364,16 +4340,40 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Fmax(L)'!$C$5:$AC$5</c:f>
+              <c:f>'Fmax(L)'!$C$5:$AK$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0.17159763313609466</c:v>
                 </c:pt>
@@ -4399,7 +4399,7 @@
                   <c:v>0.18213660245183882</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1607142857142857</c:v>
+                  <c:v>0.160714285714286</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.16626506024096388</c:v>
@@ -4411,7 +4411,7 @@
                   <c:v>0.18775510204081636</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16116504854368929</c:v>
+                  <c:v>0.16602316602316602</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.17422867513611617</c:v>
@@ -4454,6 +4454,30 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.14590747330960852</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.15662650602409633</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.15909090909090906</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.1648351648351648</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.1716738197424893</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.17437722419928825</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.17801047120418845</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.176056338028169</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.1612284069097889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8291,9 +8315,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Ben Bolen" id="{BF8D1625-453C-4F9B-90F4-27D3407028E0}" userId="S::bbolen@pdx.edu::2756ab96-c1b4-4d6e-be6a-ace1ad4a8569" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8591,20 +8613,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B1" dT="2023-12-10T07:41:58.62" personId="{BF8D1625-453C-4F9B-90F4-27D3407028E0}" id="{C0933719-F29F-4D06-A942-723E036E6640}">
-    <text>Changed resting length to 515</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5D9837-CB16-4300-A1DA-BD967A7687F8}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8813,7 +8827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0289F67D-1B36-4222-87CA-07D1B890BA50}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -9807,8 +9821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050AE67D-A238-4925-A0DE-87F77397D646}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10307,8 +10321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C902C6E6-059B-43BE-A924-BB7C80CB41D4}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10868,11 +10882,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2BFFE4-73AB-4B28-8B60-9C656B1F81F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2BFFE4-73AB-4B28-8B60-9C656B1F81F0}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10890,7 +10904,7 @@
         <v>5</v>
       </c>
       <c r="B1">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="D1" t="s">
         <v>37</v>
@@ -10917,7 +10931,7 @@
       </c>
       <c r="B3">
         <f>1-B2/B1</f>
-        <v>0.16116504854368929</v>
+        <v>0.16602316602316602</v>
       </c>
       <c r="I3" s="1"/>
       <c r="M3" s="2"/>
@@ -10957,7 +10971,7 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E26" si="0">1-A6/$B$1</f>
-        <v>0.16116504854368929</v>
+        <v>0.16602316602316602</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F26" si="1">E6/$B$3</f>
@@ -10979,11 +10993,11 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.1631067961165048</v>
+        <v>0.16795366795366795</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>1.0120481927710843</v>
+        <v>1.0116279069767442</v>
       </c>
       <c r="G7">
         <v>669</v>
@@ -11001,11 +11015,11 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.16699029126213594</v>
+        <v>0.1718146718146718</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>1.0361445783132532</v>
+        <v>1.0348837209302324</v>
       </c>
       <c r="G8">
         <v>663</v>
@@ -11026,11 +11040,11 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.14563106796116509</v>
+        <v>0.15057915057915061</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>0.90361445783132577</v>
+        <v>0.90697674418604668</v>
       </c>
       <c r="G9">
         <v>677</v>
@@ -11041,18 +11055,18 @@
         <v>515</v>
       </c>
       <c r="C10">
-        <v>443.2</v>
+        <v>427.6</v>
       </c>
       <c r="D10">
         <v>615</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.7915057915057799E-3</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.4883720930232488E-2</v>
       </c>
       <c r="G10">
         <v>755</v>
@@ -11073,11 +11087,11 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>1.747572815533982E-2</v>
+        <v>2.316602316602312E-2</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>0.10843373493975915</v>
+        <v>0.13953488372092995</v>
       </c>
       <c r="G11">
         <v>746</v>
@@ -11095,11 +11109,11 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>3.300970873786413E-2</v>
+        <v>3.8610038610038644E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>0.20481927710843409</v>
+        <v>0.23255813953488391</v>
       </c>
       <c r="G12">
         <v>737</v>
@@ -11117,11 +11131,11 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>5.0485436893203839E-2</v>
+        <v>5.5984555984555984E-2</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>0.31325301204819256</v>
+        <v>0.33720930232558138</v>
       </c>
       <c r="G13">
         <v>729</v>
@@ -11139,11 +11153,11 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>7.3786407766990303E-2</v>
+        <v>7.9150579150579103E-2</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0.45783132530120496</v>
+        <v>0.47674418604651136</v>
       </c>
       <c r="G14">
         <v>715</v>
@@ -11161,11 +11175,11 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.14757281553398061</v>
+        <v>0.15250965250965254</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0.91566265060240992</v>
+        <v>0.91860465116279089</v>
       </c>
       <c r="G15">
         <v>675</v>
@@ -11183,11 +11197,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.13009708737864079</v>
+        <v>0.13513513513513509</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0.80722891566265076</v>
+        <v>0.81395348837209269</v>
       </c>
       <c r="G16">
         <v>687</v>
@@ -11205,11 +11219,11 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0.11067961165048545</v>
+        <v>0.11583011583011582</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0.68674698795180744</v>
+        <v>0.69767441860465107</v>
       </c>
       <c r="G17">
         <v>696</v>
@@ -11227,11 +11241,11 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>9.7087378640776656E-2</v>
+        <v>0.10231660231660233</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0.6024096385542167</v>
+        <v>0.61627906976744196</v>
       </c>
       <c r="G18">
         <v>703</v>
@@ -11251,11 +11265,11 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>8.1553398058252458E-2</v>
+        <v>8.6872586872586921E-2</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0.50602409638554247</v>
+        <v>0.52325581395348864</v>
       </c>
       <c r="G19">
         <v>711</v>
@@ -11275,11 +11289,11 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-1.9417475728156219E-3</v>
+        <v>3.8610038610038533E-3</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>-1.2048192771084884E-2</v>
+        <v>2.3255813953488327E-2</v>
       </c>
       <c r="G20">
         <v>755</v>
@@ -11299,11 +11313,11 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>5.8252427184466438E-3</v>
+        <v>1.158301158301156E-2</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>3.6144578313253281E-2</v>
+        <v>6.9767441860464977E-2</v>
       </c>
       <c r="G21">
         <v>753</v>
@@ -11321,11 +11335,11 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>2.5242718446601975E-2</v>
+        <v>3.0888030888030937E-2</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>0.15662650602409661</v>
+        <v>0.18604651162790728</v>
       </c>
       <c r="G22">
         <v>742</v>
@@ -11352,11 +11366,11 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>1.3592233009708687E-2</v>
+        <v>1.9305019305019266E-2</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>8.4337349397590064E-2</v>
+        <v>0.11627906976744162</v>
       </c>
       <c r="G23">
         <v>750</v>
@@ -11374,11 +11388,11 @@
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>5.8252427184465994E-2</v>
+        <v>6.370656370656369E-2</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>0.36144578313253001</v>
+        <v>0.38372093023255804</v>
       </c>
       <c r="G24">
         <v>724</v>
@@ -11396,11 +11410,11 @@
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>4.4660194174757306E-2</v>
+        <v>5.0193050193050204E-2</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>0.27710843373493999</v>
+        <v>0.30232558139534887</v>
       </c>
       <c r="G25">
         <v>734</v>
@@ -11411,18 +11425,18 @@
         <v>518</v>
       </c>
       <c r="C26">
-        <v>518</v>
+        <v>429</v>
       </c>
       <c r="D26">
         <v>617</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>-5.8252427184466438E-3</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>-3.6144578313253281E-2</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>761</v>
@@ -11447,16 +11461,15 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CFFEA6-F038-4ADE-B4DB-050B0246E0CF}">
-  <dimension ref="A1:AC64"/>
+  <dimension ref="A1:AK64"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31:S53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11471,7 +11484,7 @@
     <col min="17" max="17" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
@@ -11529,7 +11542,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
@@ -11584,7 +11597,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -11669,8 +11682,32 @@
       <c r="AC3" s="15">
         <v>281</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AD3" s="21">
+        <v>83</v>
+      </c>
+      <c r="AE3" s="21">
+        <v>132</v>
+      </c>
+      <c r="AF3" s="21">
+        <v>182</v>
+      </c>
+      <c r="AG3" s="21">
+        <v>233</v>
+      </c>
+      <c r="AH3" s="21">
+        <v>281</v>
+      </c>
+      <c r="AI3" s="21">
+        <v>382</v>
+      </c>
+      <c r="AJ3" s="21">
+        <v>426</v>
+      </c>
+      <c r="AK3" s="21">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -11742,8 +11779,32 @@
       <c r="AC4" s="15">
         <v>240</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD4" s="21">
+        <v>70</v>
+      </c>
+      <c r="AE4" s="21">
+        <v>111</v>
+      </c>
+      <c r="AF4" s="21">
+        <v>152</v>
+      </c>
+      <c r="AG4" s="21">
+        <v>193</v>
+      </c>
+      <c r="AH4" s="21">
+        <v>232</v>
+      </c>
+      <c r="AI4" s="21">
+        <v>314</v>
+      </c>
+      <c r="AJ4" s="21">
+        <v>351</v>
+      </c>
+      <c r="AK4" s="21">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -11780,7 +11841,7 @@
         <v>0.18213660245183882</v>
       </c>
       <c r="K5" s="7">
-        <v>0.1607142857142857</v>
+        <v>0.160714285714286</v>
       </c>
       <c r="L5" s="8">
         <v>0.16626506024096388</v>
@@ -11792,7 +11853,7 @@
         <v>0.18775510204081636</v>
       </c>
       <c r="O5" s="9">
-        <v>0.16116504854368929</v>
+        <v>0.16602316602316602</v>
       </c>
       <c r="P5" s="16">
         <f t="shared" ref="P5:W5" si="2">1-P4/P3</f>
@@ -11827,7 +11888,7 @@
         <v>0.16580310880829019</v>
       </c>
       <c r="X5" s="16">
-        <f t="shared" ref="X5:AC5" si="3">1-X4/X3</f>
+        <f t="shared" ref="X5:AK5" si="3">1-X4/X3</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="Y5" s="16">
@@ -11850,8 +11911,40 @@
         <f t="shared" si="3"/>
         <v>0.14590747330960852</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AD5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.15662650602409633</v>
+      </c>
+      <c r="AE5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.15909090909090906</v>
+      </c>
+      <c r="AF5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.1648351648351648</v>
+      </c>
+      <c r="AG5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.1716738197424893</v>
+      </c>
+      <c r="AH5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.17437722419928825</v>
+      </c>
+      <c r="AI5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.17801047120418845</v>
+      </c>
+      <c r="AJ5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.176056338028169</v>
+      </c>
+      <c r="AK5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.1612284069097889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
@@ -11880,10 +11973,10 @@
         <v>461.6</v>
       </c>
       <c r="K6">
-        <v>348.58</v>
+        <v>334.74</v>
       </c>
       <c r="L6">
-        <v>459.63</v>
+        <v>445</v>
       </c>
       <c r="M6">
         <v>460</v>
@@ -11937,7 +12030,7 @@
         <v>402.48</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
@@ -12020,7 +12113,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="1" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" s="1" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -12054,7 +12147,7 @@
       <c r="R8"/>
       <c r="S8"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -12087,7 +12180,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10">
         <v>838</v>
@@ -12110,7 +12203,7 @@
         <v>1.3793103448275808E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11">
         <v>837</v>
@@ -12133,7 +12226,7 @@
         <v>2.0689655172413713E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12">
         <v>836</v>
@@ -12156,7 +12249,7 @@
         <v>2.7586206896551616E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13">
         <v>835</v>
@@ -12179,7 +12272,7 @@
         <v>3.4482758620689523E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="8">
         <v>834</v>
@@ -12212,7 +12305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -12241,13 +12334,13 @@
         <v>112</v>
       </c>
       <c r="Y15">
-        <v>334</v>
+        <v>334.74</v>
       </c>
       <c r="Z15">
         <v>0.1607142857142857</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16">
         <v>780</v>
@@ -12305,7 +12398,7 @@
         <v>455</v>
       </c>
       <c r="Y17">
-        <v>464.5</v>
+        <v>460</v>
       </c>
       <c r="Z17">
         <v>0.15824175824175823</v>
@@ -12369,7 +12462,7 @@
         <v>518</v>
       </c>
       <c r="Y19">
-        <v>490</v>
+        <v>455.83</v>
       </c>
       <c r="Z19">
         <v>0.16602316602316602</v>
@@ -12704,25 +12797,25 @@
       <c r="L31" s="14">
         <v>840</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="3">
         <v>0</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="4">
         <v>114.32</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="4">
         <v>191.8</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="4">
         <v>275.2</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="4">
         <v>355.4</v>
       </c>
-      <c r="S31" s="6">
+      <c r="S31" s="13">
         <v>447.1</v>
       </c>
       <c r="U31">
@@ -12755,22 +12848,22 @@
       <c r="L32" s="15">
         <v>780</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="5">
         <v>0</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N32" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="22">
         <v>139.19999999999999</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="22">
         <v>216</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="22">
         <v>299.7</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="22">
         <v>378.1</v>
       </c>
       <c r="S32" s="6">
@@ -12811,22 +12904,22 @@
       <c r="L33" s="15">
         <v>709</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="5">
         <v>0</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="22">
         <v>124.21</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="22">
         <v>201.4</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="22">
         <v>276.02</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="22">
         <v>355.9</v>
       </c>
       <c r="S33" s="6">
@@ -12861,22 +12954,22 @@
       <c r="L34" s="15">
         <v>571</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="5">
         <v>0</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="22">
         <v>136.1</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="22">
         <v>212.39</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="22">
         <v>288.2</v>
       </c>
-      <c r="R34">
+      <c r="R34" s="22">
         <v>366.94</v>
       </c>
       <c r="S34" s="6">
@@ -12911,26 +13004,26 @@
       <c r="L35" s="15">
         <v>112</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="5">
         <v>0</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="Q35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R35" t="s">
+      <c r="R35" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S35" s="6">
-        <v>348.58</v>
+        <v>334.74</v>
       </c>
       <c r="U35">
         <v>5</v>
@@ -12961,26 +13054,26 @@
       <c r="L36" s="15">
         <v>415</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="5">
         <v>0</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="Q36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R36" t="s">
+      <c r="R36" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S36" s="6">
-        <v>459.63</v>
+        <v>445</v>
       </c>
       <c r="U36">
         <v>6</v>
@@ -13011,22 +13104,22 @@
       <c r="L37" s="15">
         <v>455</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="5">
         <v>0</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N37" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="Q37" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R37" t="s">
+      <c r="R37" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S37" s="6">
@@ -13062,22 +13155,22 @@
       <c r="L38" s="15">
         <v>490</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="5">
         <v>0</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O38" t="s">
+      <c r="O38" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P38" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="Q38" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R38" t="s">
+      <c r="R38" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S38" s="6">
@@ -13118,22 +13211,22 @@
       <c r="L39" s="15">
         <v>518</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="5">
         <v>0</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="Q39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R39" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S39" s="6">
@@ -13168,22 +13261,22 @@
       <c r="L40" s="15">
         <v>551</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="5">
         <v>0</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="22">
         <v>129.26</v>
       </c>
-      <c r="P40">
+      <c r="P40" s="22">
         <v>201.3</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="22">
         <v>282.33999999999997</v>
       </c>
-      <c r="R40">
+      <c r="R40" s="22">
         <v>360.24</v>
       </c>
       <c r="S40" s="6">
@@ -13218,22 +13311,22 @@
       <c r="L41" s="15">
         <v>361</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="5">
         <v>0</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="22">
         <v>121.5</v>
       </c>
-      <c r="P41">
+      <c r="P41" s="22">
         <v>192.91</v>
       </c>
-      <c r="Q41">
+      <c r="Q41" s="22">
         <v>269</v>
       </c>
-      <c r="R41">
+      <c r="R41" s="22">
         <v>344.5</v>
       </c>
       <c r="S41" s="6">
@@ -13268,22 +13361,22 @@
       <c r="L42" s="15">
         <v>54</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="5">
         <v>0</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="22">
         <v>56.1</v>
       </c>
-      <c r="P42">
+      <c r="P42" s="22">
         <v>103.37</v>
       </c>
-      <c r="Q42">
+      <c r="Q42" s="22">
         <v>155.44999999999999</v>
       </c>
-      <c r="R42">
+      <c r="R42" s="22">
         <v>207</v>
       </c>
       <c r="S42" s="6">
@@ -13318,22 +13411,22 @@
       <c r="L43" s="15">
         <v>27</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="5">
         <v>0</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N43" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O43" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P43" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="Q43" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R43" t="s">
+      <c r="R43" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S43" s="6">
@@ -13369,22 +13462,22 @@
       <c r="L44" s="15">
         <v>69</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="5">
         <v>0</v>
       </c>
-      <c r="N44" t="s">
+      <c r="N44" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O44" t="s">
+      <c r="O44" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P44" t="s">
+      <c r="P44" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="Q44" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R44" t="s">
+      <c r="R44" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S44" s="6">
@@ -13425,22 +13518,22 @@
       <c r="L45" s="15">
         <v>275</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="5">
         <v>0</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N45" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O45" t="s">
+      <c r="O45" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P45" t="s">
+      <c r="P45" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="Q45" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R45" t="s">
+      <c r="R45" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S45" s="6">
@@ -13475,22 +13568,22 @@
       <c r="L46" s="15">
         <v>151</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="5">
         <v>0</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O46" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P46" t="s">
+      <c r="P46" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="Q46" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R46" t="s">
+      <c r="R46" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S46" s="6">
@@ -13525,22 +13618,22 @@
       <c r="L47" s="15">
         <v>193</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="5">
         <v>0</v>
       </c>
-      <c r="N47" t="s">
+      <c r="N47" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O47" t="s">
+      <c r="O47" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P47" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="Q47" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R47" t="s">
+      <c r="R47" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S47" s="6">
@@ -13575,22 +13668,22 @@
       <c r="L48" s="15">
         <v>10</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="5">
         <v>0</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N48" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O48" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="P48" t="s">
+      <c r="P48" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="Q48" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="R48" t="s">
+      <c r="R48" s="22" t="s">
         <v>47</v>
       </c>
       <c r="S48" s="6">
@@ -13625,22 +13718,22 @@
       <c r="L49" s="15">
         <v>120</v>
       </c>
-      <c r="M49">
+      <c r="M49" s="5">
         <v>0</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="22">
         <v>19.7</v>
       </c>
-      <c r="O49">
+      <c r="O49" s="22">
         <v>66</v>
       </c>
-      <c r="P49">
+      <c r="P49" s="22">
         <v>124.82</v>
       </c>
-      <c r="Q49">
+      <c r="Q49" s="22">
         <v>195.1</v>
       </c>
-      <c r="R49">
+      <c r="R49" s="22">
         <v>258.3</v>
       </c>
       <c r="S49" s="6">
@@ -13676,22 +13769,22 @@
       <c r="L50" s="15">
         <v>220</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="5">
         <v>0</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="22">
         <v>23</v>
       </c>
-      <c r="O50">
+      <c r="O50" s="22">
         <v>80.8</v>
       </c>
-      <c r="P50">
+      <c r="P50" s="22">
         <v>146.19999999999999</v>
       </c>
-      <c r="Q50">
+      <c r="Q50" s="22">
         <v>215.6</v>
       </c>
-      <c r="R50">
+      <c r="R50" s="22">
         <v>289.8</v>
       </c>
       <c r="S50" s="6">
@@ -13732,22 +13825,22 @@
       <c r="L51" s="15">
         <v>260</v>
       </c>
-      <c r="M51">
+      <c r="M51" s="5">
         <v>0</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="22">
         <v>31.9</v>
       </c>
-      <c r="O51">
+      <c r="O51" s="22">
         <v>89.7</v>
       </c>
-      <c r="P51">
+      <c r="P51" s="22">
         <v>154.6</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="22">
         <v>225.3</v>
       </c>
-      <c r="R51">
+      <c r="R51" s="22">
         <v>294.8</v>
       </c>
       <c r="S51" s="6">
@@ -13783,22 +13876,22 @@
       <c r="L52" s="15">
         <v>281</v>
       </c>
-      <c r="M52">
+      <c r="M52" s="5">
         <v>0</v>
       </c>
-      <c r="N52">
+      <c r="N52" s="22">
         <v>54.65</v>
       </c>
-      <c r="O52">
+      <c r="O52" s="22">
         <v>117.8</v>
       </c>
-      <c r="P52">
+      <c r="P52" s="22">
         <v>185</v>
       </c>
-      <c r="Q52">
+      <c r="Q52" s="22">
         <v>257.2</v>
       </c>
-      <c r="R52">
+      <c r="R52" s="22">
         <v>329.9</v>
       </c>
       <c r="S52" s="6">
@@ -13808,7 +13901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>9</v>
       </c>
@@ -13839,25 +13932,25 @@
       <c r="L53" s="15">
         <v>281</v>
       </c>
-      <c r="M53" s="8">
+      <c r="M53" s="5">
         <v>0</v>
       </c>
-      <c r="N53" s="8">
+      <c r="N53" s="22">
         <v>37.1</v>
       </c>
-      <c r="O53" s="8">
+      <c r="O53" s="22">
         <v>101.1</v>
       </c>
-      <c r="P53" s="8">
+      <c r="P53" s="22">
         <v>170.4</v>
       </c>
-      <c r="Q53" s="8">
+      <c r="Q53" s="22">
         <v>242.3</v>
       </c>
-      <c r="R53" s="8">
+      <c r="R53" s="22">
         <v>314.2</v>
       </c>
-      <c r="S53" s="9">
+      <c r="S53" s="6">
         <v>406</v>
       </c>
       <c r="U53">
@@ -13887,11 +13980,20 @@
         <f t="shared" si="18"/>
         <v>-8.5</v>
       </c>
-      <c r="L54" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="T54" s="2" t="s">
-        <v>48</v>
+      <c r="L54" s="21">
+        <v>83</v>
+      </c>
+      <c r="M54" s="5">
+        <v>0</v>
+      </c>
+      <c r="N54" s="22"/>
+      <c r="O54" s="22"/>
+      <c r="P54" s="22"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="22"/>
+      <c r="S54" s="6"/>
+      <c r="U54">
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
@@ -13921,6 +14023,21 @@
       </c>
       <c r="I55" t="s">
         <v>36</v>
+      </c>
+      <c r="L55" s="21">
+        <v>132</v>
+      </c>
+      <c r="M55" s="5">
+        <v>0</v>
+      </c>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
+      <c r="P55" s="22"/>
+      <c r="Q55" s="22"/>
+      <c r="R55" s="22"/>
+      <c r="S55" s="6"/>
+      <c r="U55">
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13946,6 +14063,21 @@
         <f>G56/$U$5</f>
         <v>4.2553191489361979E-2</v>
       </c>
+      <c r="L56" s="21">
+        <v>182</v>
+      </c>
+      <c r="M56" s="5">
+        <v>0</v>
+      </c>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="22"/>
+      <c r="Q56" s="22"/>
+      <c r="R56" s="22"/>
+      <c r="S56" s="6"/>
+      <c r="U56">
+        <v>26</v>
+      </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
@@ -13974,6 +14106,21 @@
       </c>
       <c r="I57" t="s">
         <v>36</v>
+      </c>
+      <c r="L57" s="21">
+        <v>233</v>
+      </c>
+      <c r="M57" s="5">
+        <v>0</v>
+      </c>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="22"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="22"/>
+      <c r="S57" s="6"/>
+      <c r="U57">
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13999,6 +14146,21 @@
         <f>G58/$V$5</f>
         <v>8.6956521739130155E-2</v>
       </c>
+      <c r="L58" s="21">
+        <v>281</v>
+      </c>
+      <c r="M58" s="5">
+        <v>0</v>
+      </c>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="6"/>
+      <c r="U58">
+        <v>28</v>
+      </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
@@ -14027,6 +14189,21 @@
       </c>
       <c r="I59" t="s">
         <v>36</v>
+      </c>
+      <c r="L59" s="21">
+        <v>382</v>
+      </c>
+      <c r="M59" s="5">
+        <v>0</v>
+      </c>
+      <c r="N59" s="22"/>
+      <c r="O59" s="22"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="22"/>
+      <c r="S59" s="6"/>
+      <c r="U59">
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14052,6 +14229,21 @@
         <f>G60/$W$5</f>
         <v>0</v>
       </c>
+      <c r="L60" s="21">
+        <v>426</v>
+      </c>
+      <c r="M60" s="5">
+        <v>0</v>
+      </c>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="22"/>
+      <c r="S60" s="6"/>
+      <c r="U60">
+        <v>30</v>
+      </c>
     </row>
     <row r="61" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
@@ -14077,6 +14269,21 @@
       <c r="H61" s="9">
         <f>G61/$X$5</f>
         <v>0</v>
+      </c>
+      <c r="L61" s="21">
+        <v>521</v>
+      </c>
+      <c r="M61" s="7">
+        <v>0</v>
+      </c>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="9"/>
+      <c r="U61">
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14101,6 +14308,12 @@
       <c r="H62" s="9">
         <f>G62/$X$5</f>
         <v>0</v>
+      </c>
+      <c r="L62" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="T62" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
GeneralizedForceFit figure and excel files
GeneralizedForceFit saved as eps and sent to Alex. Coefficient tables and straight force test finished.
</commit_message>
<xml_diff>
--- a/Testing_Data/StraightForceTest.xlsx
+++ b/Testing_Data/StraightForceTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8333DB-A609-4D46-BF25-54D4A7841DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DE5BDA-4857-4E60-92FA-50DC8D1F52BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CE45C211-BD3F-4CC7-8CF8-DB47A93DE884}"/>
   </bookViews>
   <sheets>
     <sheet name="11.2 cm, no T" sheetId="2" r:id="rId1"/>
@@ -425,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -467,7 +467,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2129,19 +2128,19 @@
                 <c:pt idx="7">
                   <c:v>461.6</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>343.29149999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>453.65</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>439.63069999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="8" formatCode="General">
+                  <c:v>334.74</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
                   <c:v>458.6</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="12" formatCode="General">
                   <c:v>455.83</c:v>
                 </c:pt>
                 <c:pt idx="13">
@@ -15380,7 +15379,7 @@
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F34" s="34">
+      <c r="F34" s="33">
         <f>F6</f>
         <v>1</v>
       </c>
@@ -15390,7 +15389,7 @@
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F35" s="34">
+      <c r="F35" s="33">
         <f t="shared" ref="F35:F51" si="3">F7</f>
         <v>0.91780821917808175</v>
       </c>
@@ -15400,7 +15399,7 @@
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F36" s="34">
+      <c r="F36" s="33">
         <f t="shared" si="3"/>
         <v>0.60273972602739745</v>
       </c>
@@ -15410,7 +15409,7 @@
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F37" s="34">
+      <c r="F37" s="33">
         <f t="shared" si="3"/>
         <v>0.84246575342465746</v>
       </c>
@@ -15420,7 +15419,7 @@
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F38" s="34">
+      <c r="F38" s="33">
         <f t="shared" si="3"/>
         <v>0.80821917808219157</v>
       </c>
@@ -15430,7 +15429,7 @@
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F39" s="34">
+      <c r="F39" s="33">
         <f t="shared" si="3"/>
         <v>0.78082191780821886</v>
       </c>
@@ -15440,7 +15439,7 @@
       </c>
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F40" s="34">
+      <c r="F40" s="33">
         <f t="shared" si="3"/>
         <v>0.65753424657534221</v>
       </c>
@@ -15450,7 +15449,7 @@
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F41" s="34">
+      <c r="F41" s="33">
         <f t="shared" si="3"/>
         <v>0.49315068493150649</v>
       </c>
@@ -15460,7 +15459,7 @@
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F42" s="34">
+      <c r="F42" s="33">
         <f t="shared" si="3"/>
         <v>0.35616438356164348</v>
       </c>
@@ -15470,7 +15469,7 @@
       </c>
     </row>
     <row r="43" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F43" s="34">
+      <c r="F43" s="33">
         <f t="shared" si="3"/>
         <v>0.20547945205479412</v>
       </c>
@@ -15480,7 +15479,7 @@
       </c>
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F44" s="34">
+      <c r="F44" s="33">
         <f t="shared" si="3"/>
         <v>0.10958904109589025</v>
       </c>
@@ -15490,7 +15489,7 @@
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F45" s="34">
+      <c r="F45" s="33">
         <f t="shared" si="3"/>
         <v>1.3698630136986368E-2</v>
       </c>
@@ -15500,7 +15499,7 @@
       </c>
     </row>
     <row r="46" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F46" s="34">
+      <c r="F46" s="33">
         <f t="shared" si="3"/>
         <v>4.1095890410959103E-2</v>
       </c>
@@ -15510,7 +15509,7 @@
       </c>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F47" s="34">
+      <c r="F47" s="33">
         <f t="shared" si="3"/>
         <v>2.7397260273972737E-2</v>
       </c>
@@ -15520,7 +15519,7 @@
       </c>
     </row>
     <row r="48" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F48" s="34">
+      <c r="F48" s="33">
         <f t="shared" si="3"/>
         <v>0.10958904109589025</v>
       </c>
@@ -15530,7 +15529,7 @@
       </c>
     </row>
     <row r="49" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F49" s="34">
+      <c r="F49" s="33">
         <f t="shared" si="3"/>
         <v>0.2602739726027396</v>
       </c>
@@ -15540,7 +15539,7 @@
       </c>
     </row>
     <row r="50" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F50" s="34">
+      <c r="F50" s="33">
         <f t="shared" si="3"/>
         <v>0.43835616438356168</v>
       </c>
@@ -15550,7 +15549,7 @@
       </c>
     </row>
     <row r="51" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F51" s="34">
+      <c r="F51" s="33">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -15570,7 +15569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C902C6E6-059B-43BE-A924-BB7C80CB41D4}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F55" sqref="F55:G55"/>
     </sheetView>
   </sheetViews>
@@ -16354,8 +16353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2BFFE4-73AB-4B28-8B60-9C656B1F81F0}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17136,8 +17135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CFFEA6-F038-4ADE-B4DB-050B0246E0CF}">
   <dimension ref="A1:AK64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="I38" workbookViewId="0">
+      <selection activeCell="S53" sqref="S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17645,19 +17644,19 @@
       <c r="J6" s="20">
         <v>461.6</v>
       </c>
-      <c r="K6" s="20">
-        <v>343.29149999999998</v>
-      </c>
-      <c r="L6" s="20">
-        <v>453.65</v>
-      </c>
-      <c r="M6" s="20">
-        <v>439.63069999999999</v>
-      </c>
-      <c r="N6" s="20">
+      <c r="K6" s="6">
+        <v>334.74</v>
+      </c>
+      <c r="L6" s="6">
+        <v>445</v>
+      </c>
+      <c r="M6" s="6">
+        <v>460</v>
+      </c>
+      <c r="N6" s="6">
         <v>458.6</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="6">
         <v>455.83</v>
       </c>
       <c r="P6" s="24">
@@ -19119,7 +19118,7 @@
         <v>207</v>
       </c>
       <c r="S42" s="6">
-        <v>266.5</v>
+        <v>238.2</v>
       </c>
       <c r="U42">
         <v>12</v>
@@ -19475,7 +19474,7 @@
       <c r="R49" s="20">
         <v>260.55869222423098</v>
       </c>
-      <c r="S49" s="21">
+      <c r="S49" s="31">
         <v>341.27196536755503</v>
       </c>
       <c r="U49">
@@ -19526,7 +19525,7 @@
       <c r="R50" s="20">
         <v>289.187518020212</v>
       </c>
-      <c r="S50" s="21">
+      <c r="S50" s="31">
         <v>377.74958573221602</v>
       </c>
       <c r="U50">
@@ -19582,7 +19581,7 @@
       <c r="R51" s="20">
         <v>296.11482667822497</v>
       </c>
-      <c r="S51" s="21">
+      <c r="S51" s="31">
         <v>383.52926262490701</v>
       </c>
       <c r="U51">
@@ -19633,7 +19632,7 @@
       <c r="R52" s="20">
         <v>330.30026824494303</v>
       </c>
-      <c r="S52" s="21">
+      <c r="S52" s="31">
         <v>419.44061252688402</v>
       </c>
       <c r="U52">
@@ -19689,7 +19688,7 @@
       <c r="R53" s="20">
         <v>317.62763704109801</v>
       </c>
-      <c r="S53" s="21">
+      <c r="S53" s="31">
         <v>407.12949095758</v>
       </c>
       <c r="U53">
@@ -19740,7 +19739,7 @@
       <c r="R54" s="20">
         <v>242.220715418238</v>
       </c>
-      <c r="S54" s="21">
+      <c r="S54" s="31">
         <v>317.15233304749597</v>
       </c>
       <c r="U54">
@@ -19796,7 +19795,7 @@
       <c r="R55" s="20">
         <v>279.78315320204098</v>
       </c>
-      <c r="S55" s="21">
+      <c r="S55" s="31">
         <v>363.613537141714</v>
       </c>
       <c r="U55">
@@ -19847,7 +19846,7 @@
       <c r="R56" s="20">
         <v>296.374690754661</v>
       </c>
-      <c r="S56" s="21">
+      <c r="S56" s="31">
         <v>380.24683840846097</v>
       </c>
       <c r="U56">
@@ -19903,7 +19902,7 @@
       <c r="R57" s="20">
         <v>310.32310380453703</v>
       </c>
-      <c r="S57" s="21">
+      <c r="S57" s="31">
         <v>394.94626968755199</v>
       </c>
       <c r="U57">
@@ -19954,7 +19953,7 @@
       <c r="R58" s="20">
         <v>345.04680550109401</v>
       </c>
-      <c r="S58" s="21">
+      <c r="S58" s="31">
         <v>436.00172829341199</v>
       </c>
       <c r="U58">
@@ -20010,7 +20009,7 @@
       <c r="R59" s="20">
         <v>364.77020715224899</v>
       </c>
-      <c r="S59" s="21">
+      <c r="S59" s="31">
         <v>459.110104683619</v>
       </c>
       <c r="U59">
@@ -20061,7 +20060,7 @@
       <c r="R60" s="20">
         <v>359.08125122058698</v>
       </c>
-      <c r="S60" s="21">
+      <c r="S60" s="31">
         <v>455.36635322123999</v>
       </c>
       <c r="U60">
@@ -20114,7 +20113,7 @@
       <c r="R61" s="32">
         <v>385.527373443047</v>
       </c>
-      <c r="S61" s="33">
+      <c r="S61" s="31">
         <v>484.22539420023401</v>
       </c>
       <c r="U61">

</xml_diff>